<commit_message>
Novas palavras - Letra B
</commit_message>
<xml_diff>
--- a/arquivo/top3000.xlsx
+++ b/arquivo/top3000.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gamer\Documents\Git\ingles\arquivo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A62DFA8-4356-4898-B731-CE6D215653B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E3BE68-1926-4C6A-B391-BA2A3AB118DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{41433B18-DF96-4E6A-98C1-9F6F4C6BB2A4}"/>
   </bookViews>
@@ -9051,7 +9051,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9086,31 +9086,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="EF Circular Latin"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="9"/>
-      <name val="EF Circular Latin"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -9120,6 +9101,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9188,7 +9175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -9197,6 +9184,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -9204,6 +9192,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -9224,28 +9215,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -9564,8 +9548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FA6857-B5B6-4301-A86D-7552E8D00242}">
   <dimension ref="A1:H3001"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A213" workbookViewId="0">
-      <selection activeCell="A223" sqref="A223:C234"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="E237" sqref="E237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9592,7 +9576,7 @@
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="11">
         <v>44997</v>
       </c>
     </row>
@@ -9603,7 +9587,7 @@
       <c r="B3" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="1">
@@ -9612,7 +9596,7 @@
       <c r="B4" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="1">
@@ -9621,7 +9605,7 @@
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" ht="15.75">
       <c r="A6" s="1">
@@ -9630,7 +9614,7 @@
       <c r="B6" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="12"/>
     </row>
     <row r="7" spans="1:3" ht="15.75">
       <c r="A7" s="1">
@@ -9639,7 +9623,7 @@
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:3" ht="15.75">
       <c r="A8" s="1">
@@ -9648,7 +9632,7 @@
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:3" ht="15.75">
       <c r="A9" s="1">
@@ -9657,7 +9641,7 @@
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:3" ht="15.75">
       <c r="A10" s="1">
@@ -9666,7 +9650,7 @@
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="12"/>
     </row>
     <row r="11" spans="1:3" ht="15.75">
       <c r="A11" s="1">
@@ -9675,7 +9659,7 @@
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="11"/>
+      <c r="C11" s="13"/>
     </row>
     <row r="12" spans="1:3" ht="15.75">
       <c r="A12" s="1">
@@ -9684,7 +9668,7 @@
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="11">
         <v>44998</v>
       </c>
     </row>
@@ -9695,7 +9679,7 @@
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="10"/>
+      <c r="C13" s="12"/>
     </row>
     <row r="14" spans="1:3" ht="15.75">
       <c r="A14" s="1">
@@ -9704,7 +9688,7 @@
       <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="10"/>
+      <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:3" ht="15.75">
       <c r="A15" s="1">
@@ -9713,7 +9697,7 @@
       <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="10"/>
+      <c r="C15" s="12"/>
     </row>
     <row r="16" spans="1:3" ht="15.75">
       <c r="A16" s="1">
@@ -9722,7 +9706,7 @@
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="10"/>
+      <c r="C16" s="12"/>
     </row>
     <row r="17" spans="1:3" ht="15.75">
       <c r="A17" s="1">
@@ -9731,7 +9715,7 @@
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="12"/>
     </row>
     <row r="18" spans="1:3" ht="15.75">
       <c r="A18" s="1">
@@ -9740,7 +9724,7 @@
       <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="10"/>
+      <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:3" ht="15.75">
       <c r="A19" s="1">
@@ -9749,7 +9733,7 @@
       <c r="B19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="10"/>
+      <c r="C19" s="12"/>
     </row>
     <row r="20" spans="1:3" ht="15.75">
       <c r="A20" s="1">
@@ -9758,7 +9742,7 @@
       <c r="B20" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C20" s="10"/>
+      <c r="C20" s="12"/>
     </row>
     <row r="21" spans="1:3" ht="15.75">
       <c r="A21" s="1">
@@ -9767,7 +9751,7 @@
       <c r="B21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="11"/>
+      <c r="C21" s="13"/>
     </row>
     <row r="22" spans="1:3" ht="15.75">
       <c r="A22" s="1">
@@ -9776,7 +9760,7 @@
       <c r="B22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="11">
         <v>44999</v>
       </c>
     </row>
@@ -9787,7 +9771,7 @@
       <c r="B23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="10"/>
+      <c r="C23" s="12"/>
     </row>
     <row r="24" spans="1:3" ht="15.75">
       <c r="A24" s="1">
@@ -9796,7 +9780,7 @@
       <c r="B24" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="10"/>
+      <c r="C24" s="12"/>
     </row>
     <row r="25" spans="1:3" ht="15.75">
       <c r="A25" s="1">
@@ -9805,7 +9789,7 @@
       <c r="B25" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="10"/>
+      <c r="C25" s="12"/>
     </row>
     <row r="26" spans="1:3" ht="15.75">
       <c r="A26" s="1">
@@ -9814,7 +9798,7 @@
       <c r="B26" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="10"/>
+      <c r="C26" s="12"/>
     </row>
     <row r="27" spans="1:3" ht="15.75">
       <c r="A27" s="1">
@@ -9823,7 +9807,7 @@
       <c r="B27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="10"/>
+      <c r="C27" s="12"/>
     </row>
     <row r="28" spans="1:3" ht="15.75">
       <c r="A28" s="1">
@@ -9832,7 +9816,7 @@
       <c r="B28" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="10"/>
+      <c r="C28" s="12"/>
     </row>
     <row r="29" spans="1:3" ht="15.75">
       <c r="A29" s="1">
@@ -9841,7 +9825,7 @@
       <c r="B29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="10"/>
+      <c r="C29" s="12"/>
     </row>
     <row r="30" spans="1:3" ht="15.75">
       <c r="A30" s="1">
@@ -9850,7 +9834,7 @@
       <c r="B30" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="10"/>
+      <c r="C30" s="12"/>
     </row>
     <row r="31" spans="1:3" ht="15.75">
       <c r="A31" s="1">
@@ -9859,7 +9843,7 @@
       <c r="B31" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="11"/>
+      <c r="C31" s="13"/>
     </row>
     <row r="32" spans="1:3" ht="15.75">
       <c r="A32" s="1">
@@ -9868,7 +9852,7 @@
       <c r="B32" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C32" s="14">
         <v>45000</v>
       </c>
     </row>
@@ -9879,7 +9863,7 @@
       <c r="B33" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="13"/>
+      <c r="C33" s="15"/>
     </row>
     <row r="34" spans="1:3" ht="15.75">
       <c r="A34" s="1">
@@ -9888,7 +9872,7 @@
       <c r="B34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="13"/>
+      <c r="C34" s="15"/>
     </row>
     <row r="35" spans="1:3" ht="15.75">
       <c r="A35" s="1">
@@ -9897,7 +9881,7 @@
       <c r="B35" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="13"/>
+      <c r="C35" s="15"/>
     </row>
     <row r="36" spans="1:3" ht="15.75">
       <c r="A36" s="1">
@@ -9906,7 +9890,7 @@
       <c r="B36" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="13"/>
+      <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" ht="15.75">
       <c r="A37" s="1">
@@ -9915,7 +9899,7 @@
       <c r="B37" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="13"/>
+      <c r="C37" s="15"/>
     </row>
     <row r="38" spans="1:3" ht="15.75">
       <c r="A38" s="1">
@@ -9924,7 +9908,7 @@
       <c r="B38" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="13"/>
+      <c r="C38" s="15"/>
     </row>
     <row r="39" spans="1:3" ht="15.75">
       <c r="A39" s="1">
@@ -9933,7 +9917,7 @@
       <c r="B39" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="13"/>
+      <c r="C39" s="15"/>
     </row>
     <row r="40" spans="1:3" ht="15.75">
       <c r="A40" s="1">
@@ -9942,7 +9926,7 @@
       <c r="B40" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="13"/>
+      <c r="C40" s="15"/>
     </row>
     <row r="41" spans="1:3" ht="15.75">
       <c r="A41" s="1">
@@ -9951,7 +9935,7 @@
       <c r="B41" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="14"/>
+      <c r="C41" s="16"/>
     </row>
     <row r="42" spans="1:3" ht="15.75">
       <c r="A42" s="1">
@@ -9960,7 +9944,7 @@
       <c r="B42" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="12">
+      <c r="C42" s="14">
         <v>45001</v>
       </c>
     </row>
@@ -9971,7 +9955,7 @@
       <c r="B43" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="13"/>
+      <c r="C43" s="15"/>
     </row>
     <row r="44" spans="1:3" ht="15.75">
       <c r="A44" s="1">
@@ -9980,7 +9964,7 @@
       <c r="B44" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="13"/>
+      <c r="C44" s="15"/>
     </row>
     <row r="45" spans="1:3" ht="15.75">
       <c r="A45" s="1">
@@ -9989,7 +9973,7 @@
       <c r="B45" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C45" s="11">
         <v>45002</v>
       </c>
     </row>
@@ -10000,7 +9984,7 @@
       <c r="B46" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C46" s="10"/>
+      <c r="C46" s="12"/>
     </row>
     <row r="47" spans="1:3" ht="15.75">
       <c r="A47" s="1">
@@ -10009,7 +9993,7 @@
       <c r="B47" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="11"/>
+      <c r="C47" s="13"/>
     </row>
     <row r="48" spans="1:3" ht="15.75">
       <c r="A48" s="1">
@@ -10018,7 +10002,7 @@
       <c r="B48" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C48" s="9">
+      <c r="C48" s="11">
         <v>45004</v>
       </c>
     </row>
@@ -10029,7 +10013,7 @@
       <c r="B49" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C49" s="10"/>
+      <c r="C49" s="12"/>
     </row>
     <row r="50" spans="1:3" ht="15.75">
       <c r="A50" s="1">
@@ -10038,7 +10022,7 @@
       <c r="B50" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C50" s="10"/>
+      <c r="C50" s="12"/>
     </row>
     <row r="51" spans="1:3" ht="15.75">
       <c r="A51" s="1">
@@ -10047,7 +10031,7 @@
       <c r="B51" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="10"/>
+      <c r="C51" s="12"/>
     </row>
     <row r="52" spans="1:3" ht="15.75">
       <c r="A52" s="1">
@@ -10056,7 +10040,7 @@
       <c r="B52" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="10"/>
+      <c r="C52" s="12"/>
     </row>
     <row r="53" spans="1:3" ht="15.75">
       <c r="A53" s="1">
@@ -10065,7 +10049,7 @@
       <c r="B53" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="11"/>
+      <c r="C53" s="13"/>
     </row>
     <row r="54" spans="1:3" ht="15.75">
       <c r="A54" s="1">
@@ -10074,7 +10058,7 @@
       <c r="B54" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="9">
+      <c r="C54" s="11">
         <v>45005</v>
       </c>
     </row>
@@ -10085,7 +10069,7 @@
       <c r="B55" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="10"/>
+      <c r="C55" s="12"/>
     </row>
     <row r="56" spans="1:3" ht="15.75">
       <c r="A56" s="1">
@@ -10094,7 +10078,7 @@
       <c r="B56" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="10"/>
+      <c r="C56" s="12"/>
     </row>
     <row r="57" spans="1:3" ht="15.75">
       <c r="A57" s="1">
@@ -10103,7 +10087,7 @@
       <c r="B57" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C57" s="10"/>
+      <c r="C57" s="12"/>
     </row>
     <row r="58" spans="1:3" ht="15.75">
       <c r="A58" s="1">
@@ -10112,7 +10096,7 @@
       <c r="B58" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C58" s="10"/>
+      <c r="C58" s="12"/>
     </row>
     <row r="59" spans="1:3" ht="15.75">
       <c r="A59" s="1">
@@ -10121,7 +10105,7 @@
       <c r="B59" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C59" s="11"/>
+      <c r="C59" s="13"/>
     </row>
     <row r="60" spans="1:3" ht="15.75">
       <c r="A60" s="1">
@@ -10130,7 +10114,7 @@
       <c r="B60" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C60" s="9">
+      <c r="C60" s="11">
         <v>45006</v>
       </c>
     </row>
@@ -10141,7 +10125,7 @@
       <c r="B61" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C61" s="10"/>
+      <c r="C61" s="12"/>
     </row>
     <row r="62" spans="1:3" ht="15.75">
       <c r="A62" s="1">
@@ -10150,7 +10134,7 @@
       <c r="B62" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C62" s="10"/>
+      <c r="C62" s="12"/>
     </row>
     <row r="63" spans="1:3" ht="15.75">
       <c r="A63" s="1">
@@ -10159,7 +10143,7 @@
       <c r="B63" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C63" s="10"/>
+      <c r="C63" s="12"/>
     </row>
     <row r="64" spans="1:3" ht="15.75">
       <c r="A64" s="1">
@@ -10168,7 +10152,7 @@
       <c r="B64" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C64" s="10"/>
+      <c r="C64" s="12"/>
     </row>
     <row r="65" spans="1:3" ht="15.75">
       <c r="A65" s="1">
@@ -10177,7 +10161,7 @@
       <c r="B65" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C65" s="11"/>
+      <c r="C65" s="13"/>
     </row>
     <row r="66" spans="1:3" ht="15.75">
       <c r="A66" s="1">
@@ -10186,7 +10170,7 @@
       <c r="B66" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C66" s="9">
+      <c r="C66" s="11">
         <v>45007</v>
       </c>
     </row>
@@ -10197,7 +10181,7 @@
       <c r="B67" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C67" s="10"/>
+      <c r="C67" s="12"/>
     </row>
     <row r="68" spans="1:3" ht="15.75">
       <c r="A68" s="1">
@@ -10206,7 +10190,7 @@
       <c r="B68" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C68" s="10"/>
+      <c r="C68" s="12"/>
     </row>
     <row r="69" spans="1:3" ht="15.75">
       <c r="A69" s="1">
@@ -10215,7 +10199,7 @@
       <c r="B69" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C69" s="10"/>
+      <c r="C69" s="12"/>
     </row>
     <row r="70" spans="1:3" ht="15.75">
       <c r="A70" s="1">
@@ -10224,7 +10208,7 @@
       <c r="B70" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C70" s="10"/>
+      <c r="C70" s="12"/>
     </row>
     <row r="71" spans="1:3" ht="15.75">
       <c r="A71" s="1">
@@ -10233,7 +10217,7 @@
       <c r="B71" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C71" s="11"/>
+      <c r="C71" s="13"/>
     </row>
     <row r="72" spans="1:3" ht="15.75">
       <c r="A72" s="1">
@@ -10242,7 +10226,7 @@
       <c r="B72" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C72" s="9">
+      <c r="C72" s="11">
         <v>45008</v>
       </c>
     </row>
@@ -10253,7 +10237,7 @@
       <c r="B73" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C73" s="10"/>
+      <c r="C73" s="12"/>
     </row>
     <row r="74" spans="1:3" ht="15.75">
       <c r="A74" s="1">
@@ -10262,7 +10246,7 @@
       <c r="B74" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C74" s="10"/>
+      <c r="C74" s="12"/>
     </row>
     <row r="75" spans="1:3" ht="15.75">
       <c r="A75" s="1">
@@ -10271,7 +10255,7 @@
       <c r="B75" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C75" s="10"/>
+      <c r="C75" s="12"/>
     </row>
     <row r="76" spans="1:3" ht="15.75">
       <c r="A76" s="1">
@@ -10280,7 +10264,7 @@
       <c r="B76" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C76" s="10"/>
+      <c r="C76" s="12"/>
     </row>
     <row r="77" spans="1:3" ht="15.75">
       <c r="A77" s="1">
@@ -10289,7 +10273,7 @@
       <c r="B77" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C77" s="11"/>
+      <c r="C77" s="13"/>
     </row>
     <row r="78" spans="1:3" ht="15.75">
       <c r="A78" s="1">
@@ -10298,7 +10282,7 @@
       <c r="B78" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C78" s="9">
+      <c r="C78" s="11">
         <v>45009</v>
       </c>
     </row>
@@ -10309,7 +10293,7 @@
       <c r="B79" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C79" s="10"/>
+      <c r="C79" s="12"/>
     </row>
     <row r="80" spans="1:3" ht="15.75">
       <c r="A80" s="1">
@@ -10318,7 +10302,7 @@
       <c r="B80" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C80" s="10"/>
+      <c r="C80" s="12"/>
     </row>
     <row r="81" spans="1:3" ht="15.75">
       <c r="A81" s="1">
@@ -10327,7 +10311,7 @@
       <c r="B81" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C81" s="10"/>
+      <c r="C81" s="12"/>
     </row>
     <row r="82" spans="1:3" ht="15.75">
       <c r="A82" s="1">
@@ -10336,7 +10320,7 @@
       <c r="B82" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C82" s="10"/>
+      <c r="C82" s="12"/>
     </row>
     <row r="83" spans="1:3" ht="15.75">
       <c r="A83" s="1">
@@ -10345,7 +10329,7 @@
       <c r="B83" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C83" s="11"/>
+      <c r="C83" s="13"/>
     </row>
     <row r="84" spans="1:3" ht="15.75">
       <c r="A84" s="1">
@@ -10354,7 +10338,7 @@
       <c r="B84" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C84" s="6">
+      <c r="C84" s="7">
         <v>45011</v>
       </c>
     </row>
@@ -10365,7 +10349,7 @@
       <c r="B85" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C85" s="7"/>
+      <c r="C85" s="8"/>
     </row>
     <row r="86" spans="1:3" ht="15.75">
       <c r="A86" s="1">
@@ -10374,7 +10358,7 @@
       <c r="B86" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C86" s="7"/>
+      <c r="C86" s="8"/>
     </row>
     <row r="87" spans="1:3" ht="15.75">
       <c r="A87" s="1">
@@ -10383,7 +10367,7 @@
       <c r="B87" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C87" s="7"/>
+      <c r="C87" s="8"/>
     </row>
     <row r="88" spans="1:3" ht="15.75">
       <c r="A88" s="1">
@@ -10392,7 +10376,7 @@
       <c r="B88" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C88" s="7"/>
+      <c r="C88" s="8"/>
     </row>
     <row r="89" spans="1:3" ht="15.75">
       <c r="A89" s="1">
@@ -10401,7 +10385,7 @@
       <c r="B89" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C89" s="8"/>
+      <c r="C89" s="9"/>
     </row>
     <row r="90" spans="1:3" ht="15.75">
       <c r="A90" s="1">
@@ -10410,7 +10394,7 @@
       <c r="B90" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C90" s="6">
+      <c r="C90" s="7">
         <v>45012</v>
       </c>
     </row>
@@ -10421,7 +10405,7 @@
       <c r="B91" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C91" s="7"/>
+      <c r="C91" s="8"/>
     </row>
     <row r="92" spans="1:3" ht="15.75">
       <c r="A92" s="1">
@@ -10430,7 +10414,7 @@
       <c r="B92" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C92" s="7"/>
+      <c r="C92" s="8"/>
     </row>
     <row r="93" spans="1:3" ht="15.75">
       <c r="A93" s="1">
@@ -10439,7 +10423,7 @@
       <c r="B93" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C93" s="7"/>
+      <c r="C93" s="8"/>
     </row>
     <row r="94" spans="1:3" ht="15.75">
       <c r="A94" s="1">
@@ -10448,7 +10432,7 @@
       <c r="B94" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C94" s="7"/>
+      <c r="C94" s="8"/>
     </row>
     <row r="95" spans="1:3" ht="15.75">
       <c r="A95" s="1">
@@ -10457,7 +10441,7 @@
       <c r="B95" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C95" s="8"/>
+      <c r="C95" s="9"/>
     </row>
     <row r="96" spans="1:3" ht="15.75">
       <c r="A96" s="1">
@@ -10466,7 +10450,7 @@
       <c r="B96" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C96" s="6">
+      <c r="C96" s="7">
         <v>45013</v>
       </c>
     </row>
@@ -10477,7 +10461,7 @@
       <c r="B97" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C97" s="7"/>
+      <c r="C97" s="8"/>
     </row>
     <row r="98" spans="1:3" ht="15.75">
       <c r="A98" s="1">
@@ -10486,7 +10470,7 @@
       <c r="B98" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C98" s="8"/>
+      <c r="C98" s="9"/>
     </row>
     <row r="99" spans="1:3" ht="15.75">
       <c r="A99" s="1">
@@ -10495,7 +10479,7 @@
       <c r="B99" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C99" s="6">
+      <c r="C99" s="7">
         <v>45014</v>
       </c>
     </row>
@@ -10506,7 +10490,7 @@
       <c r="B100" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C100" s="7"/>
+      <c r="C100" s="8"/>
     </row>
     <row r="101" spans="1:3" ht="15.75">
       <c r="A101" s="1">
@@ -10515,7 +10499,7 @@
       <c r="B101" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C101" s="8"/>
+      <c r="C101" s="9"/>
     </row>
     <row r="102" spans="1:3" ht="15.75">
       <c r="A102" s="1">
@@ -10524,7 +10508,7 @@
       <c r="B102" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C102" s="6">
+      <c r="C102" s="7">
         <v>45015</v>
       </c>
     </row>
@@ -10535,7 +10519,7 @@
       <c r="B103" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C103" s="7"/>
+      <c r="C103" s="8"/>
     </row>
     <row r="104" spans="1:3" ht="15.75">
       <c r="A104" s="1">
@@ -10544,7 +10528,7 @@
       <c r="B104" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C104" s="8"/>
+      <c r="C104" s="9"/>
     </row>
     <row r="105" spans="1:3" ht="15.75">
       <c r="A105" s="1">
@@ -10553,7 +10537,7 @@
       <c r="B105" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C105" s="6">
+      <c r="C105" s="7">
         <v>45016</v>
       </c>
     </row>
@@ -10564,7 +10548,7 @@
       <c r="B106" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C106" s="7"/>
+      <c r="C106" s="8"/>
     </row>
     <row r="107" spans="1:3" ht="15.75">
       <c r="A107" s="1">
@@ -10573,7 +10557,7 @@
       <c r="B107" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C107" s="8"/>
+      <c r="C107" s="9"/>
     </row>
     <row r="108" spans="1:3" ht="15.75">
       <c r="A108" s="1">
@@ -10582,7 +10566,7 @@
       <c r="B108" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C108" s="6">
+      <c r="C108" s="7">
         <v>45019</v>
       </c>
     </row>
@@ -10593,7 +10577,7 @@
       <c r="B109" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C109" s="7"/>
+      <c r="C109" s="8"/>
     </row>
     <row r="110" spans="1:3" ht="15.75">
       <c r="A110" s="1">
@@ -10602,7 +10586,7 @@
       <c r="B110" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C110" s="8"/>
+      <c r="C110" s="9"/>
     </row>
     <row r="111" spans="1:3" ht="15.75">
       <c r="A111" s="1">
@@ -10611,7 +10595,7 @@
       <c r="B111" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C111" s="6">
+      <c r="C111" s="7">
         <v>45020</v>
       </c>
     </row>
@@ -10622,7 +10606,7 @@
       <c r="B112" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C112" s="7"/>
+      <c r="C112" s="8"/>
     </row>
     <row r="113" spans="1:3" ht="15.75">
       <c r="A113" s="1">
@@ -10631,7 +10615,7 @@
       <c r="B113" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C113" s="8"/>
+      <c r="C113" s="9"/>
     </row>
     <row r="114" spans="1:3" ht="15.75">
       <c r="A114" s="1">
@@ -10640,7 +10624,7 @@
       <c r="B114" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C114" s="6">
+      <c r="C114" s="7">
         <v>45023</v>
       </c>
     </row>
@@ -10651,7 +10635,7 @@
       <c r="B115" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C115" s="7"/>
+      <c r="C115" s="8"/>
     </row>
     <row r="116" spans="1:3" ht="15.75">
       <c r="A116" s="1">
@@ -10660,7 +10644,7 @@
       <c r="B116" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C116" s="7"/>
+      <c r="C116" s="8"/>
     </row>
     <row r="117" spans="1:3" ht="15.75">
       <c r="A117" s="1">
@@ -10669,7 +10653,7 @@
       <c r="B117" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C117" s="7"/>
+      <c r="C117" s="8"/>
     </row>
     <row r="118" spans="1:3" ht="15.75">
       <c r="A118" s="1">
@@ -10678,7 +10662,7 @@
       <c r="B118" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="C118" s="7"/>
+      <c r="C118" s="8"/>
     </row>
     <row r="119" spans="1:3" ht="15.75">
       <c r="A119" s="1">
@@ -10687,7 +10671,7 @@
       <c r="B119" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C119" s="8"/>
+      <c r="C119" s="9"/>
     </row>
     <row r="120" spans="1:3" ht="15.75">
       <c r="A120" s="1">
@@ -10696,7 +10680,7 @@
       <c r="B120" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C120" s="6">
+      <c r="C120" s="7">
         <v>45026</v>
       </c>
     </row>
@@ -10707,7 +10691,7 @@
       <c r="B121" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C121" s="7"/>
+      <c r="C121" s="8"/>
     </row>
     <row r="122" spans="1:3" ht="15.75">
       <c r="A122" s="1">
@@ -10716,7 +10700,7 @@
       <c r="B122" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C122" s="7"/>
+      <c r="C122" s="8"/>
     </row>
     <row r="123" spans="1:3" ht="15.75">
       <c r="A123" s="1">
@@ -10725,7 +10709,7 @@
       <c r="B123" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C123" s="7"/>
+      <c r="C123" s="8"/>
     </row>
     <row r="124" spans="1:3" ht="15.75">
       <c r="A124" s="1">
@@ -10734,7 +10718,7 @@
       <c r="B124" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C124" s="7"/>
+      <c r="C124" s="8"/>
     </row>
     <row r="125" spans="1:3" ht="15.75">
       <c r="A125" s="1">
@@ -10743,7 +10727,7 @@
       <c r="B125" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C125" s="8"/>
+      <c r="C125" s="9"/>
     </row>
     <row r="126" spans="1:3" ht="15.75">
       <c r="A126" s="1">
@@ -10752,7 +10736,7 @@
       <c r="B126" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C126" s="6">
+      <c r="C126" s="7">
         <v>45027</v>
       </c>
     </row>
@@ -10763,7 +10747,7 @@
       <c r="B127" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C127" s="7"/>
+      <c r="C127" s="8"/>
     </row>
     <row r="128" spans="1:3" ht="15.75">
       <c r="A128" s="1">
@@ -10772,7 +10756,7 @@
       <c r="B128" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C128" s="7"/>
+      <c r="C128" s="8"/>
     </row>
     <row r="129" spans="1:3" ht="15.75">
       <c r="A129" s="1">
@@ -10781,7 +10765,7 @@
       <c r="B129" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C129" s="7"/>
+      <c r="C129" s="8"/>
     </row>
     <row r="130" spans="1:3" ht="15.75">
       <c r="A130" s="1">
@@ -10790,7 +10774,7 @@
       <c r="B130" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C130" s="7"/>
+      <c r="C130" s="8"/>
     </row>
     <row r="131" spans="1:3" ht="15.75">
       <c r="A131" s="1">
@@ -10799,7 +10783,7 @@
       <c r="B131" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C131" s="8"/>
+      <c r="C131" s="9"/>
     </row>
     <row r="132" spans="1:3" ht="15.75">
       <c r="A132" s="1">
@@ -10808,7 +10792,7 @@
       <c r="B132" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C132" s="6">
+      <c r="C132" s="7">
         <v>45028</v>
       </c>
     </row>
@@ -10819,7 +10803,7 @@
       <c r="B133" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C133" s="7"/>
+      <c r="C133" s="8"/>
     </row>
     <row r="134" spans="1:3" ht="15.75">
       <c r="A134" s="1">
@@ -10828,7 +10812,7 @@
       <c r="B134" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C134" s="8"/>
+      <c r="C134" s="9"/>
     </row>
     <row r="135" spans="1:3" ht="15.75">
       <c r="A135" s="1">
@@ -10837,7 +10821,7 @@
       <c r="B135" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C135" s="6">
+      <c r="C135" s="7">
         <v>45029</v>
       </c>
     </row>
@@ -10848,7 +10832,7 @@
       <c r="B136" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C136" s="7"/>
+      <c r="C136" s="8"/>
     </row>
     <row r="137" spans="1:3" ht="15.75">
       <c r="A137" s="1">
@@ -10857,7 +10841,7 @@
       <c r="B137" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C137" s="8"/>
+      <c r="C137" s="9"/>
     </row>
     <row r="138" spans="1:3" ht="15.75">
       <c r="A138" s="1">
@@ -10866,7 +10850,7 @@
       <c r="B138" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C138" s="6">
+      <c r="C138" s="7">
         <v>45030</v>
       </c>
     </row>
@@ -10877,7 +10861,7 @@
       <c r="B139" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C139" s="7"/>
+      <c r="C139" s="8"/>
     </row>
     <row r="140" spans="1:3" ht="15.75">
       <c r="A140" s="1">
@@ -10886,7 +10870,7 @@
       <c r="B140" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C140" s="8"/>
+      <c r="C140" s="9"/>
     </row>
     <row r="141" spans="1:3" ht="15.75">
       <c r="A141" s="1">
@@ -10895,7 +10879,7 @@
       <c r="B141" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C141" s="6">
+      <c r="C141" s="7">
         <v>45031</v>
       </c>
     </row>
@@ -10906,7 +10890,7 @@
       <c r="B142" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C142" s="7"/>
+      <c r="C142" s="8"/>
     </row>
     <row r="143" spans="1:3" ht="15.75">
       <c r="A143" s="1">
@@ -10915,7 +10899,7 @@
       <c r="B143" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C143" s="8"/>
+      <c r="C143" s="9"/>
     </row>
     <row r="144" spans="1:3" ht="15.75">
       <c r="A144" s="1">
@@ -10924,7 +10908,7 @@
       <c r="B144" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C144" s="6">
+      <c r="C144" s="7">
         <v>45032</v>
       </c>
     </row>
@@ -10935,7 +10919,7 @@
       <c r="B145" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C145" s="7"/>
+      <c r="C145" s="8"/>
     </row>
     <row r="146" spans="1:3" ht="15.75">
       <c r="A146" s="1">
@@ -10944,7 +10928,7 @@
       <c r="B146" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C146" s="8"/>
+      <c r="C146" s="9"/>
     </row>
     <row r="147" spans="1:3" ht="15.75">
       <c r="A147" s="1">
@@ -10953,7 +10937,7 @@
       <c r="B147" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C147" s="6">
+      <c r="C147" s="7">
         <v>45033</v>
       </c>
     </row>
@@ -10964,7 +10948,7 @@
       <c r="B148" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C148" s="7"/>
+      <c r="C148" s="8"/>
     </row>
     <row r="149" spans="1:3" ht="15.75">
       <c r="A149" s="1">
@@ -10973,7 +10957,7 @@
       <c r="B149" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C149" s="8"/>
+      <c r="C149" s="9"/>
     </row>
     <row r="150" spans="1:3" ht="15.75">
       <c r="A150" s="1">
@@ -10982,7 +10966,7 @@
       <c r="B150" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C150" s="6">
+      <c r="C150" s="7">
         <v>45034</v>
       </c>
     </row>
@@ -10993,7 +10977,7 @@
       <c r="B151" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C151" s="7"/>
+      <c r="C151" s="8"/>
     </row>
     <row r="152" spans="1:3" ht="15.75">
       <c r="A152" s="1">
@@ -11002,7 +10986,7 @@
       <c r="B152" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C152" s="8"/>
+      <c r="C152" s="9"/>
     </row>
     <row r="153" spans="1:3" ht="15.75">
       <c r="A153" s="1">
@@ -11011,7 +10995,7 @@
       <c r="B153" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C153" s="6">
+      <c r="C153" s="7">
         <v>45035</v>
       </c>
     </row>
@@ -11022,7 +11006,7 @@
       <c r="B154" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C154" s="7"/>
+      <c r="C154" s="8"/>
     </row>
     <row r="155" spans="1:3" ht="15.75">
       <c r="A155" s="1">
@@ -11031,7 +11015,7 @@
       <c r="B155" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C155" s="8"/>
+      <c r="C155" s="9"/>
     </row>
     <row r="156" spans="1:3" ht="15.75">
       <c r="A156" s="1">
@@ -11040,7 +11024,7 @@
       <c r="B156" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C156" s="15"/>
+      <c r="C156" s="10"/>
     </row>
     <row r="157" spans="1:3" ht="15.75">
       <c r="A157" s="1">
@@ -11049,7 +11033,7 @@
       <c r="B157" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C157" s="7"/>
+      <c r="C157" s="8"/>
     </row>
     <row r="158" spans="1:3" ht="15.75">
       <c r="A158" s="1">
@@ -11058,7 +11042,7 @@
       <c r="B158" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C158" s="8"/>
+      <c r="C158" s="9"/>
     </row>
     <row r="159" spans="1:3" ht="15.75">
       <c r="A159" s="1">
@@ -11067,7 +11051,7 @@
       <c r="B159" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C159" s="15"/>
+      <c r="C159" s="10"/>
     </row>
     <row r="160" spans="1:3" ht="15.75">
       <c r="A160" s="1">
@@ -11076,7 +11060,7 @@
       <c r="B160" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C160" s="7"/>
+      <c r="C160" s="8"/>
     </row>
     <row r="161" spans="1:3" ht="15.75">
       <c r="A161" s="1">
@@ -11085,7 +11069,7 @@
       <c r="B161" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C161" s="8"/>
+      <c r="C161" s="9"/>
     </row>
     <row r="162" spans="1:3" ht="15.75">
       <c r="A162" s="1">
@@ -11094,7 +11078,7 @@
       <c r="B162" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C162" s="15"/>
+      <c r="C162" s="10"/>
     </row>
     <row r="163" spans="1:3" ht="15.75">
       <c r="A163" s="1">
@@ -11103,7 +11087,7 @@
       <c r="B163" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C163" s="7"/>
+      <c r="C163" s="8"/>
     </row>
     <row r="164" spans="1:3" ht="15.75">
       <c r="A164" s="1">
@@ -11112,7 +11096,7 @@
       <c r="B164" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C164" s="8"/>
+      <c r="C164" s="9"/>
     </row>
     <row r="165" spans="1:3" ht="15.75">
       <c r="A165" s="1">
@@ -11121,7 +11105,7 @@
       <c r="B165" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C165" s="15"/>
+      <c r="C165" s="10"/>
     </row>
     <row r="166" spans="1:3" ht="15.75">
       <c r="A166" s="1">
@@ -11130,7 +11114,7 @@
       <c r="B166" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C166" s="7"/>
+      <c r="C166" s="8"/>
     </row>
     <row r="167" spans="1:3" ht="15.75">
       <c r="A167" s="1">
@@ -11139,7 +11123,7 @@
       <c r="B167" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C167" s="8"/>
+      <c r="C167" s="9"/>
     </row>
     <row r="168" spans="1:3" ht="15.75">
       <c r="A168" s="1">
@@ -11148,7 +11132,7 @@
       <c r="B168" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C168" s="15"/>
+      <c r="C168" s="10"/>
     </row>
     <row r="169" spans="1:3" ht="15.75">
       <c r="A169" s="1">
@@ -11157,7 +11141,7 @@
       <c r="B169" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C169" s="7"/>
+      <c r="C169" s="8"/>
     </row>
     <row r="170" spans="1:3" ht="15.75">
       <c r="A170" s="1">
@@ -11166,7 +11150,7 @@
       <c r="B170" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C170" s="8"/>
+      <c r="C170" s="9"/>
     </row>
     <row r="171" spans="1:3" ht="15.75">
       <c r="A171" s="1">
@@ -11175,7 +11159,7 @@
       <c r="B171" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C171" s="6">
+      <c r="C171" s="7">
         <v>45041</v>
       </c>
     </row>
@@ -11186,7 +11170,7 @@
       <c r="B172" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C172" s="7"/>
+      <c r="C172" s="8"/>
     </row>
     <row r="173" spans="1:3" ht="15.75">
       <c r="A173" s="1">
@@ -11195,7 +11179,7 @@
       <c r="B173" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C173" s="8"/>
+      <c r="C173" s="9"/>
     </row>
     <row r="174" spans="1:3" ht="15.75">
       <c r="A174" s="1">
@@ -11204,7 +11188,7 @@
       <c r="B174" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C174" s="15"/>
+      <c r="C174" s="10"/>
     </row>
     <row r="175" spans="1:3" ht="15.75">
       <c r="A175" s="1">
@@ -11213,7 +11197,7 @@
       <c r="B175" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C175" s="7"/>
+      <c r="C175" s="8"/>
     </row>
     <row r="176" spans="1:3" ht="15.75">
       <c r="A176" s="1">
@@ -11222,7 +11206,7 @@
       <c r="B176" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C176" s="8"/>
+      <c r="C176" s="9"/>
     </row>
     <row r="177" spans="1:8" ht="15.75">
       <c r="A177" s="1">
@@ -11231,7 +11215,7 @@
       <c r="B177" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C177" s="15"/>
+      <c r="C177" s="10"/>
     </row>
     <row r="178" spans="1:8" ht="15.75">
       <c r="A178" s="1">
@@ -11240,7 +11224,7 @@
       <c r="B178" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C178" s="7"/>
+      <c r="C178" s="8"/>
     </row>
     <row r="179" spans="1:8" ht="15.75">
       <c r="A179" s="1">
@@ -11249,7 +11233,7 @@
       <c r="B179" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C179" s="8"/>
+      <c r="C179" s="9"/>
     </row>
     <row r="180" spans="1:8" ht="15.75">
       <c r="A180" s="1">
@@ -11258,7 +11242,7 @@
       <c r="B180" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C180" s="6">
+      <c r="C180" s="7">
         <v>45044</v>
       </c>
     </row>
@@ -11269,7 +11253,7 @@
       <c r="B181" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C181" s="7"/>
+      <c r="C181" s="8"/>
     </row>
     <row r="182" spans="1:8" ht="15.75">
       <c r="A182" s="1">
@@ -11278,7 +11262,7 @@
       <c r="B182" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C182" s="8"/>
+      <c r="C182" s="9"/>
     </row>
     <row r="183" spans="1:8" ht="15.75">
       <c r="A183" s="1">
@@ -11287,7 +11271,7 @@
       <c r="B183" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C183" s="6"/>
+      <c r="C183" s="7"/>
     </row>
     <row r="184" spans="1:8" ht="15.75">
       <c r="A184" s="1">
@@ -11296,7 +11280,7 @@
       <c r="B184" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C184" s="7"/>
+      <c r="C184" s="8"/>
     </row>
     <row r="185" spans="1:8" ht="15.75">
       <c r="A185" s="1">
@@ -11305,7 +11289,7 @@
       <c r="B185" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C185" s="8"/>
+      <c r="C185" s="9"/>
     </row>
     <row r="186" spans="1:8" ht="15.75">
       <c r="A186" s="1">
@@ -11314,7 +11298,7 @@
       <c r="B186" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C186" s="6"/>
+      <c r="C186" s="7"/>
     </row>
     <row r="187" spans="1:8" ht="15.75">
       <c r="A187" s="1">
@@ -11323,7 +11307,7 @@
       <c r="B187" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C187" s="7"/>
+      <c r="C187" s="8"/>
     </row>
     <row r="188" spans="1:8" ht="15.75">
       <c r="A188" s="1">
@@ -11332,7 +11316,7 @@
       <c r="B188" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C188" s="8"/>
+      <c r="C188" s="9"/>
       <c r="H188" s="5"/>
     </row>
     <row r="189" spans="1:8" ht="15.75">
@@ -11342,7 +11326,7 @@
       <c r="B189" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C189" s="6"/>
+      <c r="C189" s="7"/>
     </row>
     <row r="190" spans="1:8" ht="15.75">
       <c r="A190" s="1">
@@ -11351,7 +11335,7 @@
       <c r="B190" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C190" s="7"/>
+      <c r="C190" s="8"/>
     </row>
     <row r="191" spans="1:8" ht="15.75">
       <c r="A191" s="1">
@@ -11360,7 +11344,7 @@
       <c r="B191" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C191" s="8"/>
+      <c r="C191" s="9"/>
     </row>
     <row r="192" spans="1:8" ht="15.75">
       <c r="A192" s="1">
@@ -11369,7 +11353,7 @@
       <c r="B192" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C192" s="6"/>
+      <c r="C192" s="7"/>
     </row>
     <row r="193" spans="1:3" ht="15.75">
       <c r="A193" s="1">
@@ -11378,7 +11362,7 @@
       <c r="B193" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C193" s="7"/>
+      <c r="C193" s="8"/>
     </row>
     <row r="194" spans="1:3" ht="15.75">
       <c r="A194" s="1">
@@ -11387,7 +11371,7 @@
       <c r="B194" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C194" s="8"/>
+      <c r="C194" s="9"/>
     </row>
     <row r="195" spans="1:3" ht="15.75">
       <c r="A195" s="1">
@@ -11396,7 +11380,7 @@
       <c r="B195" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C195" s="6"/>
+      <c r="C195" s="7"/>
     </row>
     <row r="196" spans="1:3" ht="15.75">
       <c r="A196" s="1">
@@ -11405,7 +11389,7 @@
       <c r="B196" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C196" s="7"/>
+      <c r="C196" s="8"/>
     </row>
     <row r="197" spans="1:3" ht="15.75">
       <c r="A197" s="1">
@@ -11414,7 +11398,7 @@
       <c r="B197" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C197" s="8"/>
+      <c r="C197" s="9"/>
     </row>
     <row r="198" spans="1:3" ht="15.75">
       <c r="A198" s="1">
@@ -11423,7 +11407,7 @@
       <c r="B198" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C198" s="6"/>
+      <c r="C198" s="7"/>
     </row>
     <row r="199" spans="1:3" ht="15.75">
       <c r="A199" s="1">
@@ -11432,7 +11416,7 @@
       <c r="B199" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C199" s="7"/>
+      <c r="C199" s="8"/>
     </row>
     <row r="200" spans="1:3" ht="15.75">
       <c r="A200" s="1">
@@ -11441,7 +11425,7 @@
       <c r="B200" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C200" s="8"/>
+      <c r="C200" s="9"/>
     </row>
     <row r="201" spans="1:3" ht="15.75">
       <c r="A201" s="1">
@@ -11450,7 +11434,7 @@
       <c r="B201" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C201" s="6">
+      <c r="C201" s="7">
         <v>45051</v>
       </c>
     </row>
@@ -11461,7 +11445,7 @@
       <c r="B202" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C202" s="7"/>
+      <c r="C202" s="8"/>
     </row>
     <row r="203" spans="1:3" ht="15.75">
       <c r="A203" s="1">
@@ -11470,7 +11454,7 @@
       <c r="B203" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C203" s="8"/>
+      <c r="C203" s="9"/>
     </row>
     <row r="204" spans="1:3" ht="15.75">
       <c r="A204" s="1">
@@ -11479,7 +11463,7 @@
       <c r="B204" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C204" s="6">
+      <c r="C204" s="7">
         <v>45052</v>
       </c>
     </row>
@@ -11490,7 +11474,7 @@
       <c r="B205" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C205" s="7"/>
+      <c r="C205" s="8"/>
     </row>
     <row r="206" spans="1:3" ht="15.75">
       <c r="A206" s="1">
@@ -11499,7 +11483,7 @@
       <c r="B206" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C206" s="8"/>
+      <c r="C206" s="9"/>
     </row>
     <row r="207" spans="1:3" ht="15.75">
       <c r="A207" s="1">
@@ -11508,7 +11492,7 @@
       <c r="B207" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C207" s="6">
+      <c r="C207" s="7">
         <v>45053</v>
       </c>
     </row>
@@ -11519,7 +11503,7 @@
       <c r="B208" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C208" s="7"/>
+      <c r="C208" s="8"/>
     </row>
     <row r="209" spans="1:3" ht="15.75">
       <c r="A209" s="1">
@@ -11528,7 +11512,7 @@
       <c r="B209" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C209" s="8"/>
+      <c r="C209" s="9"/>
     </row>
     <row r="210" spans="1:3" ht="15.75">
       <c r="A210" s="1">
@@ -11537,7 +11521,7 @@
       <c r="B210" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C210" s="6">
+      <c r="C210" s="7">
         <v>45054</v>
       </c>
     </row>
@@ -11548,7 +11532,7 @@
       <c r="B211" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C211" s="7"/>
+      <c r="C211" s="8"/>
     </row>
     <row r="212" spans="1:3" ht="15.75">
       <c r="A212" s="1">
@@ -11557,7 +11541,7 @@
       <c r="B212" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C212" s="8"/>
+      <c r="C212" s="9"/>
     </row>
     <row r="213" spans="1:3" ht="15.75">
       <c r="A213" s="1">
@@ -11566,7 +11550,7 @@
       <c r="B213" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C213" s="6"/>
+      <c r="C213" s="7"/>
     </row>
     <row r="214" spans="1:3" ht="15.75">
       <c r="A214" s="1">
@@ -11575,7 +11559,7 @@
       <c r="B214" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C214" s="7"/>
+      <c r="C214" s="8"/>
     </row>
     <row r="215" spans="1:3" ht="15.75">
       <c r="A215" s="1">
@@ -11584,7 +11568,7 @@
       <c r="B215" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C215" s="8"/>
+      <c r="C215" s="9"/>
     </row>
     <row r="216" spans="1:3" ht="15.75">
       <c r="A216" s="1">
@@ -11593,7 +11577,7 @@
       <c r="B216" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C216" s="6">
+      <c r="C216" s="7">
         <v>45056</v>
       </c>
     </row>
@@ -11604,7 +11588,7 @@
       <c r="B217" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C217" s="7"/>
+      <c r="C217" s="8"/>
     </row>
     <row r="218" spans="1:3" ht="15.75">
       <c r="A218" s="1">
@@ -11613,170 +11597,170 @@
       <c r="B218" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C218" s="8"/>
+      <c r="C218" s="9"/>
     </row>
     <row r="219" spans="1:3" ht="15.75">
-      <c r="A219" s="1">
+      <c r="A219" s="18">
         <v>218</v>
       </c>
-      <c r="B219" s="19" t="s">
+      <c r="B219" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C219" s="16">
+      <c r="C219" s="19">
         <v>45057</v>
       </c>
     </row>
     <row r="220" spans="1:3" ht="15.75">
-      <c r="A220" s="1">
+      <c r="A220" s="18">
         <v>219</v>
       </c>
-      <c r="B220" s="19" t="s">
+      <c r="B220" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="C220" s="17"/>
+      <c r="C220" s="20"/>
     </row>
     <row r="221" spans="1:3" ht="15.75">
-      <c r="A221" s="1">
+      <c r="A221" s="18">
         <v>220</v>
       </c>
-      <c r="B221" s="19" t="s">
+      <c r="B221" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="C221" s="17"/>
+      <c r="C221" s="20"/>
     </row>
     <row r="222" spans="1:3" ht="15.75">
-      <c r="A222" s="1">
+      <c r="A222" s="18">
         <v>221</v>
       </c>
-      <c r="B222" s="19" t="s">
+      <c r="B222" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="C222" s="18"/>
+      <c r="C222" s="21"/>
     </row>
     <row r="223" spans="1:3" ht="15.75">
-      <c r="A223" s="21">
+      <c r="A223" s="18">
         <v>222</v>
       </c>
-      <c r="B223" s="20" t="s">
+      <c r="B223" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="C223" s="22">
+      <c r="C223" s="19">
         <v>45058</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="15.75">
-      <c r="A224" s="21">
+      <c r="A224" s="18">
         <v>223</v>
       </c>
-      <c r="B224" s="20" t="s">
+      <c r="B224" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="C224" s="23"/>
+      <c r="C224" s="22"/>
     </row>
     <row r="225" spans="1:3" ht="15.75">
-      <c r="A225" s="21">
+      <c r="A225" s="18">
         <v>224</v>
       </c>
-      <c r="B225" s="20" t="s">
+      <c r="B225" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C225" s="24"/>
+      <c r="C225" s="23"/>
     </row>
     <row r="226" spans="1:3" ht="15.75">
-      <c r="A226" s="21">
+      <c r="A226" s="18">
         <v>225</v>
       </c>
-      <c r="B226" s="20" t="s">
+      <c r="B226" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="C226" s="22">
+      <c r="C226" s="19">
         <v>45059</v>
       </c>
     </row>
     <row r="227" spans="1:3" ht="15.75">
-      <c r="A227" s="21">
+      <c r="A227" s="18">
         <v>226</v>
       </c>
-      <c r="B227" s="20" t="s">
+      <c r="B227" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="C227" s="23"/>
+      <c r="C227" s="22"/>
     </row>
     <row r="228" spans="1:3" ht="15.75">
-      <c r="A228" s="21">
+      <c r="A228" s="18">
         <v>227</v>
       </c>
-      <c r="B228" s="20" t="s">
+      <c r="B228" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="C228" s="24"/>
+      <c r="C228" s="23"/>
     </row>
     <row r="229" spans="1:3" ht="15.75">
-      <c r="A229" s="21">
+      <c r="A229" s="18">
         <v>228</v>
       </c>
-      <c r="B229" s="20" t="s">
+      <c r="B229" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="C229" s="22">
+      <c r="C229" s="19">
         <v>45060</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="15.75">
-      <c r="A230" s="21">
+      <c r="A230" s="18">
         <v>229</v>
       </c>
-      <c r="B230" s="20" t="s">
+      <c r="B230" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="C230" s="23"/>
+      <c r="C230" s="22"/>
     </row>
     <row r="231" spans="1:3" ht="15.75">
-      <c r="A231" s="21">
+      <c r="A231" s="18">
         <v>230</v>
       </c>
-      <c r="B231" s="20" t="s">
+      <c r="B231" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="C231" s="24"/>
+      <c r="C231" s="23"/>
     </row>
     <row r="232" spans="1:3" ht="15.75">
-      <c r="A232" s="21">
+      <c r="A232" s="18">
         <v>231</v>
       </c>
-      <c r="B232" s="20" t="s">
+      <c r="B232" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="C232" s="22">
+      <c r="C232" s="19">
         <v>45061</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="15.75">
-      <c r="A233" s="21">
+      <c r="A233" s="18">
         <v>232</v>
       </c>
-      <c r="B233" s="20" t="s">
+      <c r="B233" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="C233" s="23"/>
+      <c r="C233" s="22"/>
     </row>
     <row r="234" spans="1:3" ht="15.75">
-      <c r="A234" s="21">
+      <c r="A234" s="18">
         <v>233</v>
       </c>
-      <c r="B234" s="20" t="s">
+      <c r="B234" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="C234" s="24"/>
+      <c r="C234" s="23"/>
     </row>
     <row r="235" spans="1:3" ht="15.75">
       <c r="A235" s="1">
         <v>234</v>
       </c>
-      <c r="B235" s="2" t="s">
+      <c r="B235" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="C235" s="6">
+      <c r="C235" s="7">
         <v>45062</v>
       </c>
     </row>
@@ -11784,28 +11768,28 @@
       <c r="A236" s="1">
         <v>235</v>
       </c>
-      <c r="B236" s="2" t="s">
+      <c r="B236" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="C236" s="7"/>
+      <c r="C236" s="8"/>
     </row>
     <row r="237" spans="1:3" ht="15.75">
       <c r="A237" s="1">
         <v>236</v>
       </c>
-      <c r="B237" s="2" t="s">
+      <c r="B237" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="C237" s="8"/>
+      <c r="C237" s="9"/>
     </row>
     <row r="238" spans="1:3" ht="15.75">
       <c r="A238" s="1">
         <v>237</v>
       </c>
-      <c r="B238" s="2" t="s">
+      <c r="B238" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="C238" s="6">
+      <c r="C238" s="7">
         <v>45063</v>
       </c>
     </row>
@@ -11813,28 +11797,28 @@
       <c r="A239" s="1">
         <v>238</v>
       </c>
-      <c r="B239" s="2" t="s">
+      <c r="B239" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="C239" s="7"/>
+      <c r="C239" s="8"/>
     </row>
     <row r="240" spans="1:3" ht="15.75">
       <c r="A240" s="1">
         <v>239</v>
       </c>
-      <c r="B240" s="2" t="s">
+      <c r="B240" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="C240" s="8"/>
+      <c r="C240" s="9"/>
     </row>
     <row r="241" spans="1:3" ht="15.75">
       <c r="A241" s="1">
         <v>240</v>
       </c>
-      <c r="B241" s="2" t="s">
+      <c r="B241" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="C241" s="6">
+      <c r="C241" s="7">
         <v>45064</v>
       </c>
     </row>
@@ -11842,19 +11826,19 @@
       <c r="A242" s="1">
         <v>241</v>
       </c>
-      <c r="B242" s="2" t="s">
+      <c r="B242" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="C242" s="7"/>
+      <c r="C242" s="8"/>
     </row>
     <row r="243" spans="1:3" ht="15.75">
       <c r="A243" s="1">
         <v>242</v>
       </c>
-      <c r="B243" s="2" t="s">
+      <c r="B243" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="C243" s="8"/>
+      <c r="C243" s="9"/>
     </row>
     <row r="244" spans="1:3" ht="15.75">
       <c r="A244" s="1">
@@ -11863,7 +11847,7 @@
       <c r="B244" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="C244" s="6">
+      <c r="C244" s="7">
         <v>45065</v>
       </c>
     </row>
@@ -11874,7 +11858,7 @@
       <c r="B245" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C245" s="7"/>
+      <c r="C245" s="8"/>
     </row>
     <row r="246" spans="1:3" ht="15.75">
       <c r="A246" s="1">
@@ -11883,7 +11867,7 @@
       <c r="B246" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="C246" s="8"/>
+      <c r="C246" s="9"/>
     </row>
     <row r="247" spans="1:3" ht="15.75">
       <c r="A247" s="1">
@@ -11892,7 +11876,7 @@
       <c r="B247" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="C247" s="6">
+      <c r="C247" s="7">
         <v>45066</v>
       </c>
     </row>
@@ -11903,7 +11887,7 @@
       <c r="B248" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="C248" s="7"/>
+      <c r="C248" s="8"/>
     </row>
     <row r="249" spans="1:3" ht="15.75">
       <c r="A249" s="1">
@@ -11912,7 +11896,7 @@
       <c r="B249" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C249" s="8"/>
+      <c r="C249" s="9"/>
     </row>
     <row r="250" spans="1:3" ht="15.75">
       <c r="A250" s="1">
@@ -11921,7 +11905,7 @@
       <c r="B250" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C250" s="6">
+      <c r="C250" s="7">
         <v>45067</v>
       </c>
     </row>
@@ -11932,7 +11916,7 @@
       <c r="B251" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="C251" s="7"/>
+      <c r="C251" s="8"/>
     </row>
     <row r="252" spans="1:3" ht="15.75">
       <c r="A252" s="1">
@@ -11941,7 +11925,7 @@
       <c r="B252" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="C252" s="8"/>
+      <c r="C252" s="9"/>
     </row>
     <row r="253" spans="1:3" ht="15.75">
       <c r="A253" s="1">
@@ -11950,7 +11934,7 @@
       <c r="B253" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="C253" s="6">
+      <c r="C253" s="7">
         <v>45068</v>
       </c>
     </row>
@@ -11961,7 +11945,7 @@
       <c r="B254" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C254" s="7"/>
+      <c r="C254" s="8"/>
     </row>
     <row r="255" spans="1:3" ht="15.75">
       <c r="A255" s="1">
@@ -11970,7 +11954,7 @@
       <c r="B255" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="C255" s="8"/>
+      <c r="C255" s="9"/>
     </row>
     <row r="256" spans="1:3" ht="15.75">
       <c r="A256" s="1">
@@ -11979,7 +11963,7 @@
       <c r="B256" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="C256" s="6">
+      <c r="C256" s="7">
         <v>45069</v>
       </c>
     </row>
@@ -11990,7 +11974,7 @@
       <c r="B257" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C257" s="7"/>
+      <c r="C257" s="8"/>
     </row>
     <row r="258" spans="1:3" ht="15.75">
       <c r="A258" s="1">
@@ -11999,7 +11983,7 @@
       <c r="B258" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="C258" s="8"/>
+      <c r="C258" s="9"/>
     </row>
     <row r="259" spans="1:3" ht="15.75">
       <c r="A259" s="1">
@@ -12008,7 +11992,7 @@
       <c r="B259" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="C259" s="6">
+      <c r="C259" s="7">
         <v>45070</v>
       </c>
     </row>
@@ -12019,7 +12003,7 @@
       <c r="B260" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="C260" s="7"/>
+      <c r="C260" s="8"/>
     </row>
     <row r="261" spans="1:3" ht="15.75">
       <c r="A261" s="1">
@@ -12028,7 +12012,7 @@
       <c r="B261" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="C261" s="8"/>
+      <c r="C261" s="9"/>
     </row>
     <row r="262" spans="1:3" ht="15.75">
       <c r="A262" s="1">
@@ -12037,7 +12021,7 @@
       <c r="B262" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C262" s="6">
+      <c r="C262" s="7">
         <v>45071</v>
       </c>
     </row>
@@ -12048,7 +12032,7 @@
       <c r="B263" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C263" s="7"/>
+      <c r="C263" s="8"/>
     </row>
     <row r="264" spans="1:3" ht="15.75">
       <c r="A264" s="1">
@@ -12057,7 +12041,7 @@
       <c r="B264" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C264" s="8"/>
+      <c r="C264" s="9"/>
     </row>
     <row r="265" spans="1:3" ht="15.75">
       <c r="A265" s="1">
@@ -12066,7 +12050,7 @@
       <c r="B265" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C265" s="6">
+      <c r="C265" s="7">
         <v>45072</v>
       </c>
     </row>
@@ -12077,7 +12061,7 @@
       <c r="B266" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C266" s="7"/>
+      <c r="C266" s="8"/>
     </row>
     <row r="267" spans="1:3" ht="15.75">
       <c r="A267" s="1">
@@ -12086,7 +12070,7 @@
       <c r="B267" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C267" s="8"/>
+      <c r="C267" s="9"/>
     </row>
     <row r="268" spans="1:3" ht="15.75">
       <c r="A268" s="1">
@@ -12095,7 +12079,7 @@
       <c r="B268" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="C268" s="6">
+      <c r="C268" s="7">
         <v>45073</v>
       </c>
     </row>
@@ -12106,7 +12090,7 @@
       <c r="B269" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="C269" s="7"/>
+      <c r="C269" s="8"/>
     </row>
     <row r="270" spans="1:3" ht="15.75">
       <c r="A270" s="1">
@@ -12115,7 +12099,7 @@
       <c r="B270" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C270" s="8"/>
+      <c r="C270" s="9"/>
     </row>
     <row r="271" spans="1:3" ht="15.75">
       <c r="A271" s="1">
@@ -12124,7 +12108,7 @@
       <c r="B271" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="C271" s="6">
+      <c r="C271" s="7">
         <v>45074</v>
       </c>
     </row>
@@ -12135,7 +12119,7 @@
       <c r="B272" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C272" s="7"/>
+      <c r="C272" s="8"/>
     </row>
     <row r="273" spans="1:3" ht="15.75">
       <c r="A273" s="1">
@@ -12144,7 +12128,7 @@
       <c r="B273" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C273" s="8"/>
+      <c r="C273" s="9"/>
     </row>
     <row r="274" spans="1:3" ht="15.75">
       <c r="A274" s="1">
@@ -12153,7 +12137,7 @@
       <c r="B274" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="C274" s="6">
+      <c r="C274" s="7">
         <v>45075</v>
       </c>
     </row>
@@ -12164,7 +12148,7 @@
       <c r="B275" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C275" s="7"/>
+      <c r="C275" s="8"/>
     </row>
     <row r="276" spans="1:3" ht="15.75">
       <c r="A276" s="1">
@@ -12173,7 +12157,7 @@
       <c r="B276" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="C276" s="8"/>
+      <c r="C276" s="9"/>
     </row>
     <row r="277" spans="1:3" ht="15.75">
       <c r="A277" s="1">
@@ -12182,7 +12166,7 @@
       <c r="B277" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="C277" s="6">
+      <c r="C277" s="7">
         <v>45076</v>
       </c>
     </row>
@@ -12193,7 +12177,7 @@
       <c r="B278" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C278" s="7"/>
+      <c r="C278" s="8"/>
     </row>
     <row r="279" spans="1:3" ht="15.75">
       <c r="A279" s="1">
@@ -12202,7 +12186,7 @@
       <c r="B279" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C279" s="8"/>
+      <c r="C279" s="9"/>
     </row>
     <row r="280" spans="1:3" ht="15.75">
       <c r="A280" s="1">
@@ -12211,7 +12195,7 @@
       <c r="B280" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="C280" s="6">
+      <c r="C280" s="7">
         <v>45077</v>
       </c>
     </row>
@@ -12222,7 +12206,7 @@
       <c r="B281" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C281" s="7"/>
+      <c r="C281" s="8"/>
     </row>
     <row r="282" spans="1:3" ht="15.75">
       <c r="A282" s="1">
@@ -12231,7 +12215,7 @@
       <c r="B282" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C282" s="8"/>
+      <c r="C282" s="9"/>
     </row>
     <row r="283" spans="1:3" ht="15.75">
       <c r="A283" s="1">
@@ -12240,7 +12224,7 @@
       <c r="B283" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C283" s="6">
+      <c r="C283" s="7">
         <v>45078</v>
       </c>
     </row>
@@ -12251,7 +12235,7 @@
       <c r="B284" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="C284" s="7"/>
+      <c r="C284" s="8"/>
     </row>
     <row r="285" spans="1:3" ht="15.75">
       <c r="A285" s="1">
@@ -12260,7 +12244,7 @@
       <c r="B285" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C285" s="8"/>
+      <c r="C285" s="9"/>
     </row>
     <row r="286" spans="1:3" ht="15.75">
       <c r="A286" s="1">
@@ -12269,7 +12253,7 @@
       <c r="B286" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="C286" s="6">
+      <c r="C286" s="7">
         <v>45079</v>
       </c>
     </row>
@@ -12280,7 +12264,7 @@
       <c r="B287" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="C287" s="7"/>
+      <c r="C287" s="8"/>
     </row>
     <row r="288" spans="1:3" ht="15.75">
       <c r="A288" s="1">
@@ -12289,7 +12273,7 @@
       <c r="B288" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="C288" s="8"/>
+      <c r="C288" s="9"/>
     </row>
     <row r="289" spans="1:3" ht="15.75">
       <c r="A289" s="1">
@@ -12298,7 +12282,7 @@
       <c r="B289" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C289" s="6">
+      <c r="C289" s="7">
         <v>45080</v>
       </c>
     </row>
@@ -12309,7 +12293,7 @@
       <c r="B290" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C290" s="7"/>
+      <c r="C290" s="8"/>
     </row>
     <row r="291" spans="1:3" ht="15.75">
       <c r="A291" s="1">
@@ -12318,7 +12302,7 @@
       <c r="B291" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="C291" s="8"/>
+      <c r="C291" s="9"/>
     </row>
     <row r="292" spans="1:3" ht="15.75">
       <c r="A292" s="1">
@@ -12327,7 +12311,7 @@
       <c r="B292" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="C292" s="6">
+      <c r="C292" s="7">
         <v>45081</v>
       </c>
     </row>
@@ -12338,7 +12322,7 @@
       <c r="B293" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="C293" s="7"/>
+      <c r="C293" s="8"/>
     </row>
     <row r="294" spans="1:3" ht="15.75">
       <c r="A294" s="1">
@@ -12347,7 +12331,7 @@
       <c r="B294" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C294" s="8"/>
+      <c r="C294" s="9"/>
     </row>
     <row r="295" spans="1:3" ht="15.75">
       <c r="A295" s="1">
@@ -12356,7 +12340,7 @@
       <c r="B295" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C295" s="6">
+      <c r="C295" s="7">
         <v>45082</v>
       </c>
     </row>
@@ -12367,7 +12351,7 @@
       <c r="B296" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="C296" s="7"/>
+      <c r="C296" s="8"/>
     </row>
     <row r="297" spans="1:3" ht="15.75">
       <c r="A297" s="1">
@@ -12376,7 +12360,7 @@
       <c r="B297" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="C297" s="8"/>
+      <c r="C297" s="9"/>
     </row>
     <row r="298" spans="1:3" ht="15.75">
       <c r="A298" s="1">
@@ -12385,7 +12369,7 @@
       <c r="B298" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="C298" s="6">
+      <c r="C298" s="7">
         <v>45083</v>
       </c>
     </row>
@@ -12396,7 +12380,7 @@
       <c r="B299" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C299" s="7"/>
+      <c r="C299" s="8"/>
     </row>
     <row r="300" spans="1:3" ht="15.75">
       <c r="A300" s="1">
@@ -12405,7 +12389,7 @@
       <c r="B300" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C300" s="8"/>
+      <c r="C300" s="9"/>
     </row>
     <row r="301" spans="1:3" ht="15.75">
       <c r="A301" s="1">
@@ -36718,23 +36702,52 @@
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="C295:C297"/>
-    <mergeCell ref="C298:C300"/>
-    <mergeCell ref="C280:C282"/>
-    <mergeCell ref="C283:C285"/>
-    <mergeCell ref="C286:C288"/>
-    <mergeCell ref="C289:C291"/>
-    <mergeCell ref="C292:C294"/>
-    <mergeCell ref="C265:C267"/>
-    <mergeCell ref="C268:C270"/>
-    <mergeCell ref="C271:C273"/>
-    <mergeCell ref="C274:C276"/>
-    <mergeCell ref="C277:C279"/>
-    <mergeCell ref="C250:C252"/>
-    <mergeCell ref="C253:C255"/>
-    <mergeCell ref="C256:C258"/>
-    <mergeCell ref="C259:C261"/>
-    <mergeCell ref="C262:C264"/>
+    <mergeCell ref="C238:C240"/>
+    <mergeCell ref="C241:C243"/>
+    <mergeCell ref="C244:C246"/>
+    <mergeCell ref="C247:C249"/>
+    <mergeCell ref="C223:C225"/>
+    <mergeCell ref="C226:C228"/>
+    <mergeCell ref="C229:C231"/>
+    <mergeCell ref="C232:C234"/>
+    <mergeCell ref="C235:C237"/>
+    <mergeCell ref="C120:C125"/>
+    <mergeCell ref="C111:C113"/>
+    <mergeCell ref="C138:C140"/>
+    <mergeCell ref="C141:C143"/>
+    <mergeCell ref="C135:C137"/>
+    <mergeCell ref="C126:C131"/>
+    <mergeCell ref="C132:C134"/>
+    <mergeCell ref="C108:C110"/>
+    <mergeCell ref="C105:C107"/>
+    <mergeCell ref="C102:C104"/>
+    <mergeCell ref="C99:C101"/>
+    <mergeCell ref="C114:C119"/>
+    <mergeCell ref="C48:C53"/>
+    <mergeCell ref="C96:C98"/>
+    <mergeCell ref="C90:C95"/>
+    <mergeCell ref="C84:C89"/>
+    <mergeCell ref="C78:C83"/>
+    <mergeCell ref="C72:C77"/>
+    <mergeCell ref="C66:C71"/>
+    <mergeCell ref="C60:C65"/>
+    <mergeCell ref="C54:C59"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="C12:C21"/>
+    <mergeCell ref="C22:C31"/>
+    <mergeCell ref="C32:C41"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="C153:C155"/>
+    <mergeCell ref="C144:C146"/>
+    <mergeCell ref="C150:C152"/>
+    <mergeCell ref="C147:C149"/>
+    <mergeCell ref="C171:C173"/>
+    <mergeCell ref="C156:C158"/>
+    <mergeCell ref="C159:C161"/>
+    <mergeCell ref="C162:C164"/>
+    <mergeCell ref="C165:C167"/>
+    <mergeCell ref="C168:C170"/>
     <mergeCell ref="C219:C222"/>
     <mergeCell ref="C204:C206"/>
     <mergeCell ref="C207:C209"/>
@@ -36751,52 +36764,23 @@
     <mergeCell ref="C195:C197"/>
     <mergeCell ref="C213:C215"/>
     <mergeCell ref="C216:C218"/>
-    <mergeCell ref="C153:C155"/>
-    <mergeCell ref="C144:C146"/>
-    <mergeCell ref="C150:C152"/>
-    <mergeCell ref="C147:C149"/>
-    <mergeCell ref="C171:C173"/>
-    <mergeCell ref="C156:C158"/>
-    <mergeCell ref="C159:C161"/>
-    <mergeCell ref="C162:C164"/>
-    <mergeCell ref="C165:C167"/>
-    <mergeCell ref="C168:C170"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="C2:C11"/>
-    <mergeCell ref="C12:C21"/>
-    <mergeCell ref="C22:C31"/>
-    <mergeCell ref="C32:C41"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="C48:C53"/>
-    <mergeCell ref="C96:C98"/>
-    <mergeCell ref="C90:C95"/>
-    <mergeCell ref="C84:C89"/>
-    <mergeCell ref="C78:C83"/>
-    <mergeCell ref="C72:C77"/>
-    <mergeCell ref="C66:C71"/>
-    <mergeCell ref="C60:C65"/>
-    <mergeCell ref="C54:C59"/>
-    <mergeCell ref="C108:C110"/>
-    <mergeCell ref="C105:C107"/>
-    <mergeCell ref="C102:C104"/>
-    <mergeCell ref="C99:C101"/>
-    <mergeCell ref="C114:C119"/>
-    <mergeCell ref="C120:C125"/>
-    <mergeCell ref="C111:C113"/>
-    <mergeCell ref="C138:C140"/>
-    <mergeCell ref="C141:C143"/>
-    <mergeCell ref="C135:C137"/>
-    <mergeCell ref="C126:C131"/>
-    <mergeCell ref="C132:C134"/>
-    <mergeCell ref="C238:C240"/>
-    <mergeCell ref="C241:C243"/>
-    <mergeCell ref="C244:C246"/>
-    <mergeCell ref="C247:C249"/>
-    <mergeCell ref="C223:C225"/>
-    <mergeCell ref="C226:C228"/>
-    <mergeCell ref="C229:C231"/>
-    <mergeCell ref="C232:C234"/>
-    <mergeCell ref="C235:C237"/>
+    <mergeCell ref="C250:C252"/>
+    <mergeCell ref="C253:C255"/>
+    <mergeCell ref="C256:C258"/>
+    <mergeCell ref="C259:C261"/>
+    <mergeCell ref="C262:C264"/>
+    <mergeCell ref="C265:C267"/>
+    <mergeCell ref="C268:C270"/>
+    <mergeCell ref="C271:C273"/>
+    <mergeCell ref="C274:C276"/>
+    <mergeCell ref="C277:C279"/>
+    <mergeCell ref="C295:C297"/>
+    <mergeCell ref="C298:C300"/>
+    <mergeCell ref="C280:C282"/>
+    <mergeCell ref="C283:C285"/>
+    <mergeCell ref="C286:C288"/>
+    <mergeCell ref="C289:C291"/>
+    <mergeCell ref="C292:C294"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Novas palavras com B
</commit_message>
<xml_diff>
--- a/arquivo/top3000.xlsx
+++ b/arquivo/top3000.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gamer\Documents\Git\ingles\arquivo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E3BE68-1926-4C6A-B391-BA2A3AB118DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542337CE-F8CF-4D5B-AE32-93E46707A3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{41433B18-DF96-4E6A-98C1-9F6F4C6BB2A4}"/>
   </bookViews>
@@ -9091,7 +9091,7 @@
       <name val="EF Circular Latin"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -9107,6 +9107,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9175,7 +9187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -9185,6 +9197,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -9192,9 +9205,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -9215,23 +9225,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9548,8 +9552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FA6857-B5B6-4301-A86D-7552E8D00242}">
   <dimension ref="A1:H3001"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A235" workbookViewId="0">
-      <selection activeCell="E237" sqref="E237"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A246" workbookViewId="0">
+      <selection activeCell="B253" sqref="B253:B261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10338,7 +10342,7 @@
       <c r="B84" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C84" s="7">
+      <c r="C84" s="8">
         <v>45011</v>
       </c>
     </row>
@@ -10349,7 +10353,7 @@
       <c r="B85" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C85" s="8"/>
+      <c r="C85" s="9"/>
     </row>
     <row r="86" spans="1:3" ht="15.75">
       <c r="A86" s="1">
@@ -10358,7 +10362,7 @@
       <c r="B86" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C86" s="8"/>
+      <c r="C86" s="9"/>
     </row>
     <row r="87" spans="1:3" ht="15.75">
       <c r="A87" s="1">
@@ -10367,7 +10371,7 @@
       <c r="B87" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C87" s="8"/>
+      <c r="C87" s="9"/>
     </row>
     <row r="88" spans="1:3" ht="15.75">
       <c r="A88" s="1">
@@ -10376,7 +10380,7 @@
       <c r="B88" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C88" s="8"/>
+      <c r="C88" s="9"/>
     </row>
     <row r="89" spans="1:3" ht="15.75">
       <c r="A89" s="1">
@@ -10385,7 +10389,7 @@
       <c r="B89" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C89" s="9"/>
+      <c r="C89" s="10"/>
     </row>
     <row r="90" spans="1:3" ht="15.75">
       <c r="A90" s="1">
@@ -10394,7 +10398,7 @@
       <c r="B90" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C90" s="7">
+      <c r="C90" s="8">
         <v>45012</v>
       </c>
     </row>
@@ -10405,7 +10409,7 @@
       <c r="B91" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C91" s="8"/>
+      <c r="C91" s="9"/>
     </row>
     <row r="92" spans="1:3" ht="15.75">
       <c r="A92" s="1">
@@ -10414,7 +10418,7 @@
       <c r="B92" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C92" s="8"/>
+      <c r="C92" s="9"/>
     </row>
     <row r="93" spans="1:3" ht="15.75">
       <c r="A93" s="1">
@@ -10423,7 +10427,7 @@
       <c r="B93" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C93" s="8"/>
+      <c r="C93" s="9"/>
     </row>
     <row r="94" spans="1:3" ht="15.75">
       <c r="A94" s="1">
@@ -10432,7 +10436,7 @@
       <c r="B94" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C94" s="8"/>
+      <c r="C94" s="9"/>
     </row>
     <row r="95" spans="1:3" ht="15.75">
       <c r="A95" s="1">
@@ -10441,7 +10445,7 @@
       <c r="B95" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C95" s="9"/>
+      <c r="C95" s="10"/>
     </row>
     <row r="96" spans="1:3" ht="15.75">
       <c r="A96" s="1">
@@ -10450,7 +10454,7 @@
       <c r="B96" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C96" s="7">
+      <c r="C96" s="8">
         <v>45013</v>
       </c>
     </row>
@@ -10461,7 +10465,7 @@
       <c r="B97" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C97" s="8"/>
+      <c r="C97" s="9"/>
     </row>
     <row r="98" spans="1:3" ht="15.75">
       <c r="A98" s="1">
@@ -10470,7 +10474,7 @@
       <c r="B98" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C98" s="9"/>
+      <c r="C98" s="10"/>
     </row>
     <row r="99" spans="1:3" ht="15.75">
       <c r="A99" s="1">
@@ -10479,7 +10483,7 @@
       <c r="B99" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C99" s="7">
+      <c r="C99" s="8">
         <v>45014</v>
       </c>
     </row>
@@ -10490,7 +10494,7 @@
       <c r="B100" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C100" s="8"/>
+      <c r="C100" s="9"/>
     </row>
     <row r="101" spans="1:3" ht="15.75">
       <c r="A101" s="1">
@@ -10499,7 +10503,7 @@
       <c r="B101" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C101" s="9"/>
+      <c r="C101" s="10"/>
     </row>
     <row r="102" spans="1:3" ht="15.75">
       <c r="A102" s="1">
@@ -10508,7 +10512,7 @@
       <c r="B102" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C102" s="7">
+      <c r="C102" s="8">
         <v>45015</v>
       </c>
     </row>
@@ -10519,7 +10523,7 @@
       <c r="B103" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C103" s="8"/>
+      <c r="C103" s="9"/>
     </row>
     <row r="104" spans="1:3" ht="15.75">
       <c r="A104" s="1">
@@ -10528,7 +10532,7 @@
       <c r="B104" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C104" s="9"/>
+      <c r="C104" s="10"/>
     </row>
     <row r="105" spans="1:3" ht="15.75">
       <c r="A105" s="1">
@@ -10537,7 +10541,7 @@
       <c r="B105" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C105" s="7">
+      <c r="C105" s="8">
         <v>45016</v>
       </c>
     </row>
@@ -10548,7 +10552,7 @@
       <c r="B106" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C106" s="8"/>
+      <c r="C106" s="9"/>
     </row>
     <row r="107" spans="1:3" ht="15.75">
       <c r="A107" s="1">
@@ -10557,7 +10561,7 @@
       <c r="B107" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C107" s="9"/>
+      <c r="C107" s="10"/>
     </row>
     <row r="108" spans="1:3" ht="15.75">
       <c r="A108" s="1">
@@ -10566,7 +10570,7 @@
       <c r="B108" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C108" s="7">
+      <c r="C108" s="8">
         <v>45019</v>
       </c>
     </row>
@@ -10577,7 +10581,7 @@
       <c r="B109" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C109" s="8"/>
+      <c r="C109" s="9"/>
     </row>
     <row r="110" spans="1:3" ht="15.75">
       <c r="A110" s="1">
@@ -10586,7 +10590,7 @@
       <c r="B110" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C110" s="9"/>
+      <c r="C110" s="10"/>
     </row>
     <row r="111" spans="1:3" ht="15.75">
       <c r="A111" s="1">
@@ -10595,7 +10599,7 @@
       <c r="B111" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C111" s="7">
+      <c r="C111" s="8">
         <v>45020</v>
       </c>
     </row>
@@ -10606,7 +10610,7 @@
       <c r="B112" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C112" s="8"/>
+      <c r="C112" s="9"/>
     </row>
     <row r="113" spans="1:3" ht="15.75">
       <c r="A113" s="1">
@@ -10615,7 +10619,7 @@
       <c r="B113" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C113" s="9"/>
+      <c r="C113" s="10"/>
     </row>
     <row r="114" spans="1:3" ht="15.75">
       <c r="A114" s="1">
@@ -10624,7 +10628,7 @@
       <c r="B114" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C114" s="7">
+      <c r="C114" s="8">
         <v>45023</v>
       </c>
     </row>
@@ -10635,7 +10639,7 @@
       <c r="B115" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C115" s="8"/>
+      <c r="C115" s="9"/>
     </row>
     <row r="116" spans="1:3" ht="15.75">
       <c r="A116" s="1">
@@ -10644,7 +10648,7 @@
       <c r="B116" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C116" s="8"/>
+      <c r="C116" s="9"/>
     </row>
     <row r="117" spans="1:3" ht="15.75">
       <c r="A117" s="1">
@@ -10653,7 +10657,7 @@
       <c r="B117" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C117" s="8"/>
+      <c r="C117" s="9"/>
     </row>
     <row r="118" spans="1:3" ht="15.75">
       <c r="A118" s="1">
@@ -10662,7 +10666,7 @@
       <c r="B118" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="C118" s="8"/>
+      <c r="C118" s="9"/>
     </row>
     <row r="119" spans="1:3" ht="15.75">
       <c r="A119" s="1">
@@ -10671,7 +10675,7 @@
       <c r="B119" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C119" s="9"/>
+      <c r="C119" s="10"/>
     </row>
     <row r="120" spans="1:3" ht="15.75">
       <c r="A120" s="1">
@@ -10680,7 +10684,7 @@
       <c r="B120" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C120" s="7">
+      <c r="C120" s="8">
         <v>45026</v>
       </c>
     </row>
@@ -10691,7 +10695,7 @@
       <c r="B121" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C121" s="8"/>
+      <c r="C121" s="9"/>
     </row>
     <row r="122" spans="1:3" ht="15.75">
       <c r="A122" s="1">
@@ -10700,7 +10704,7 @@
       <c r="B122" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C122" s="8"/>
+      <c r="C122" s="9"/>
     </row>
     <row r="123" spans="1:3" ht="15.75">
       <c r="A123" s="1">
@@ -10709,7 +10713,7 @@
       <c r="B123" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C123" s="8"/>
+      <c r="C123" s="9"/>
     </row>
     <row r="124" spans="1:3" ht="15.75">
       <c r="A124" s="1">
@@ -10718,7 +10722,7 @@
       <c r="B124" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C124" s="8"/>
+      <c r="C124" s="9"/>
     </row>
     <row r="125" spans="1:3" ht="15.75">
       <c r="A125" s="1">
@@ -10727,7 +10731,7 @@
       <c r="B125" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C125" s="9"/>
+      <c r="C125" s="10"/>
     </row>
     <row r="126" spans="1:3" ht="15.75">
       <c r="A126" s="1">
@@ -10736,7 +10740,7 @@
       <c r="B126" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C126" s="7">
+      <c r="C126" s="8">
         <v>45027</v>
       </c>
     </row>
@@ -10747,7 +10751,7 @@
       <c r="B127" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C127" s="8"/>
+      <c r="C127" s="9"/>
     </row>
     <row r="128" spans="1:3" ht="15.75">
       <c r="A128" s="1">
@@ -10756,7 +10760,7 @@
       <c r="B128" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C128" s="8"/>
+      <c r="C128" s="9"/>
     </row>
     <row r="129" spans="1:3" ht="15.75">
       <c r="A129" s="1">
@@ -10765,7 +10769,7 @@
       <c r="B129" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C129" s="8"/>
+      <c r="C129" s="9"/>
     </row>
     <row r="130" spans="1:3" ht="15.75">
       <c r="A130" s="1">
@@ -10774,7 +10778,7 @@
       <c r="B130" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C130" s="8"/>
+      <c r="C130" s="9"/>
     </row>
     <row r="131" spans="1:3" ht="15.75">
       <c r="A131" s="1">
@@ -10783,7 +10787,7 @@
       <c r="B131" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C131" s="9"/>
+      <c r="C131" s="10"/>
     </row>
     <row r="132" spans="1:3" ht="15.75">
       <c r="A132" s="1">
@@ -10792,7 +10796,7 @@
       <c r="B132" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C132" s="7">
+      <c r="C132" s="8">
         <v>45028</v>
       </c>
     </row>
@@ -10803,7 +10807,7 @@
       <c r="B133" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C133" s="8"/>
+      <c r="C133" s="9"/>
     </row>
     <row r="134" spans="1:3" ht="15.75">
       <c r="A134" s="1">
@@ -10812,7 +10816,7 @@
       <c r="B134" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C134" s="9"/>
+      <c r="C134" s="10"/>
     </row>
     <row r="135" spans="1:3" ht="15.75">
       <c r="A135" s="1">
@@ -10821,7 +10825,7 @@
       <c r="B135" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C135" s="7">
+      <c r="C135" s="8">
         <v>45029</v>
       </c>
     </row>
@@ -10832,7 +10836,7 @@
       <c r="B136" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C136" s="8"/>
+      <c r="C136" s="9"/>
     </row>
     <row r="137" spans="1:3" ht="15.75">
       <c r="A137" s="1">
@@ -10841,7 +10845,7 @@
       <c r="B137" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C137" s="9"/>
+      <c r="C137" s="10"/>
     </row>
     <row r="138" spans="1:3" ht="15.75">
       <c r="A138" s="1">
@@ -10850,7 +10854,7 @@
       <c r="B138" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C138" s="7">
+      <c r="C138" s="8">
         <v>45030</v>
       </c>
     </row>
@@ -10861,7 +10865,7 @@
       <c r="B139" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C139" s="8"/>
+      <c r="C139" s="9"/>
     </row>
     <row r="140" spans="1:3" ht="15.75">
       <c r="A140" s="1">
@@ -10870,7 +10874,7 @@
       <c r="B140" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C140" s="9"/>
+      <c r="C140" s="10"/>
     </row>
     <row r="141" spans="1:3" ht="15.75">
       <c r="A141" s="1">
@@ -10879,7 +10883,7 @@
       <c r="B141" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C141" s="7">
+      <c r="C141" s="8">
         <v>45031</v>
       </c>
     </row>
@@ -10890,7 +10894,7 @@
       <c r="B142" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C142" s="8"/>
+      <c r="C142" s="9"/>
     </row>
     <row r="143" spans="1:3" ht="15.75">
       <c r="A143" s="1">
@@ -10899,7 +10903,7 @@
       <c r="B143" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C143" s="9"/>
+      <c r="C143" s="10"/>
     </row>
     <row r="144" spans="1:3" ht="15.75">
       <c r="A144" s="1">
@@ -10908,7 +10912,7 @@
       <c r="B144" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C144" s="7">
+      <c r="C144" s="8">
         <v>45032</v>
       </c>
     </row>
@@ -10919,7 +10923,7 @@
       <c r="B145" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C145" s="8"/>
+      <c r="C145" s="9"/>
     </row>
     <row r="146" spans="1:3" ht="15.75">
       <c r="A146" s="1">
@@ -10928,7 +10932,7 @@
       <c r="B146" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C146" s="9"/>
+      <c r="C146" s="10"/>
     </row>
     <row r="147" spans="1:3" ht="15.75">
       <c r="A147" s="1">
@@ -10937,7 +10941,7 @@
       <c r="B147" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C147" s="7">
+      <c r="C147" s="8">
         <v>45033</v>
       </c>
     </row>
@@ -10948,7 +10952,7 @@
       <c r="B148" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C148" s="8"/>
+      <c r="C148" s="9"/>
     </row>
     <row r="149" spans="1:3" ht="15.75">
       <c r="A149" s="1">
@@ -10957,7 +10961,7 @@
       <c r="B149" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C149" s="9"/>
+      <c r="C149" s="10"/>
     </row>
     <row r="150" spans="1:3" ht="15.75">
       <c r="A150" s="1">
@@ -10966,7 +10970,7 @@
       <c r="B150" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C150" s="7">
+      <c r="C150" s="8">
         <v>45034</v>
       </c>
     </row>
@@ -10977,7 +10981,7 @@
       <c r="B151" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C151" s="8"/>
+      <c r="C151" s="9"/>
     </row>
     <row r="152" spans="1:3" ht="15.75">
       <c r="A152" s="1">
@@ -10986,7 +10990,7 @@
       <c r="B152" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C152" s="9"/>
+      <c r="C152" s="10"/>
     </row>
     <row r="153" spans="1:3" ht="15.75">
       <c r="A153" s="1">
@@ -10995,7 +10999,7 @@
       <c r="B153" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C153" s="7">
+      <c r="C153" s="8">
         <v>45035</v>
       </c>
     </row>
@@ -11006,7 +11010,7 @@
       <c r="B154" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C154" s="8"/>
+      <c r="C154" s="9"/>
     </row>
     <row r="155" spans="1:3" ht="15.75">
       <c r="A155" s="1">
@@ -11015,7 +11019,7 @@
       <c r="B155" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C155" s="9"/>
+      <c r="C155" s="10"/>
     </row>
     <row r="156" spans="1:3" ht="15.75">
       <c r="A156" s="1">
@@ -11024,7 +11028,7 @@
       <c r="B156" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C156" s="10"/>
+      <c r="C156" s="17"/>
     </row>
     <row r="157" spans="1:3" ht="15.75">
       <c r="A157" s="1">
@@ -11033,7 +11037,7 @@
       <c r="B157" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C157" s="8"/>
+      <c r="C157" s="9"/>
     </row>
     <row r="158" spans="1:3" ht="15.75">
       <c r="A158" s="1">
@@ -11042,7 +11046,7 @@
       <c r="B158" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C158" s="9"/>
+      <c r="C158" s="10"/>
     </row>
     <row r="159" spans="1:3" ht="15.75">
       <c r="A159" s="1">
@@ -11051,7 +11055,7 @@
       <c r="B159" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C159" s="10"/>
+      <c r="C159" s="17"/>
     </row>
     <row r="160" spans="1:3" ht="15.75">
       <c r="A160" s="1">
@@ -11060,7 +11064,7 @@
       <c r="B160" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C160" s="8"/>
+      <c r="C160" s="9"/>
     </row>
     <row r="161" spans="1:3" ht="15.75">
       <c r="A161" s="1">
@@ -11069,7 +11073,7 @@
       <c r="B161" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C161" s="9"/>
+      <c r="C161" s="10"/>
     </row>
     <row r="162" spans="1:3" ht="15.75">
       <c r="A162" s="1">
@@ -11078,7 +11082,7 @@
       <c r="B162" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C162" s="10"/>
+      <c r="C162" s="17"/>
     </row>
     <row r="163" spans="1:3" ht="15.75">
       <c r="A163" s="1">
@@ -11087,7 +11091,7 @@
       <c r="B163" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C163" s="8"/>
+      <c r="C163" s="9"/>
     </row>
     <row r="164" spans="1:3" ht="15.75">
       <c r="A164" s="1">
@@ -11096,7 +11100,7 @@
       <c r="B164" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C164" s="9"/>
+      <c r="C164" s="10"/>
     </row>
     <row r="165" spans="1:3" ht="15.75">
       <c r="A165" s="1">
@@ -11105,7 +11109,7 @@
       <c r="B165" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C165" s="10"/>
+      <c r="C165" s="17"/>
     </row>
     <row r="166" spans="1:3" ht="15.75">
       <c r="A166" s="1">
@@ -11114,7 +11118,7 @@
       <c r="B166" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C166" s="8"/>
+      <c r="C166" s="9"/>
     </row>
     <row r="167" spans="1:3" ht="15.75">
       <c r="A167" s="1">
@@ -11123,7 +11127,7 @@
       <c r="B167" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C167" s="9"/>
+      <c r="C167" s="10"/>
     </row>
     <row r="168" spans="1:3" ht="15.75">
       <c r="A168" s="1">
@@ -11132,7 +11136,7 @@
       <c r="B168" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C168" s="10"/>
+      <c r="C168" s="17"/>
     </row>
     <row r="169" spans="1:3" ht="15.75">
       <c r="A169" s="1">
@@ -11141,7 +11145,7 @@
       <c r="B169" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C169" s="8"/>
+      <c r="C169" s="9"/>
     </row>
     <row r="170" spans="1:3" ht="15.75">
       <c r="A170" s="1">
@@ -11150,7 +11154,7 @@
       <c r="B170" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C170" s="9"/>
+      <c r="C170" s="10"/>
     </row>
     <row r="171" spans="1:3" ht="15.75">
       <c r="A171" s="1">
@@ -11159,7 +11163,7 @@
       <c r="B171" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C171" s="7">
+      <c r="C171" s="8">
         <v>45041</v>
       </c>
     </row>
@@ -11170,7 +11174,7 @@
       <c r="B172" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C172" s="8"/>
+      <c r="C172" s="9"/>
     </row>
     <row r="173" spans="1:3" ht="15.75">
       <c r="A173" s="1">
@@ -11179,7 +11183,7 @@
       <c r="B173" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C173" s="9"/>
+      <c r="C173" s="10"/>
     </row>
     <row r="174" spans="1:3" ht="15.75">
       <c r="A174" s="1">
@@ -11188,7 +11192,7 @@
       <c r="B174" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C174" s="10"/>
+      <c r="C174" s="17"/>
     </row>
     <row r="175" spans="1:3" ht="15.75">
       <c r="A175" s="1">
@@ -11197,7 +11201,7 @@
       <c r="B175" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C175" s="8"/>
+      <c r="C175" s="9"/>
     </row>
     <row r="176" spans="1:3" ht="15.75">
       <c r="A176" s="1">
@@ -11206,7 +11210,7 @@
       <c r="B176" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C176" s="9"/>
+      <c r="C176" s="10"/>
     </row>
     <row r="177" spans="1:8" ht="15.75">
       <c r="A177" s="1">
@@ -11215,7 +11219,7 @@
       <c r="B177" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C177" s="10"/>
+      <c r="C177" s="17"/>
     </row>
     <row r="178" spans="1:8" ht="15.75">
       <c r="A178" s="1">
@@ -11224,7 +11228,7 @@
       <c r="B178" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C178" s="8"/>
+      <c r="C178" s="9"/>
     </row>
     <row r="179" spans="1:8" ht="15.75">
       <c r="A179" s="1">
@@ -11233,7 +11237,7 @@
       <c r="B179" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C179" s="9"/>
+      <c r="C179" s="10"/>
     </row>
     <row r="180" spans="1:8" ht="15.75">
       <c r="A180" s="1">
@@ -11242,7 +11246,7 @@
       <c r="B180" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C180" s="7">
+      <c r="C180" s="8">
         <v>45044</v>
       </c>
     </row>
@@ -11253,7 +11257,7 @@
       <c r="B181" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C181" s="8"/>
+      <c r="C181" s="9"/>
     </row>
     <row r="182" spans="1:8" ht="15.75">
       <c r="A182" s="1">
@@ -11262,7 +11266,7 @@
       <c r="B182" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C182" s="9"/>
+      <c r="C182" s="10"/>
     </row>
     <row r="183" spans="1:8" ht="15.75">
       <c r="A183" s="1">
@@ -11271,7 +11275,7 @@
       <c r="B183" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C183" s="7"/>
+      <c r="C183" s="8"/>
     </row>
     <row r="184" spans="1:8" ht="15.75">
       <c r="A184" s="1">
@@ -11280,7 +11284,7 @@
       <c r="B184" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C184" s="8"/>
+      <c r="C184" s="9"/>
     </row>
     <row r="185" spans="1:8" ht="15.75">
       <c r="A185" s="1">
@@ -11289,7 +11293,7 @@
       <c r="B185" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C185" s="9"/>
+      <c r="C185" s="10"/>
     </row>
     <row r="186" spans="1:8" ht="15.75">
       <c r="A186" s="1">
@@ -11298,7 +11302,7 @@
       <c r="B186" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C186" s="7"/>
+      <c r="C186" s="8"/>
     </row>
     <row r="187" spans="1:8" ht="15.75">
       <c r="A187" s="1">
@@ -11307,7 +11311,7 @@
       <c r="B187" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C187" s="8"/>
+      <c r="C187" s="9"/>
     </row>
     <row r="188" spans="1:8" ht="15.75">
       <c r="A188" s="1">
@@ -11316,7 +11320,7 @@
       <c r="B188" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C188" s="9"/>
+      <c r="C188" s="10"/>
       <c r="H188" s="5"/>
     </row>
     <row r="189" spans="1:8" ht="15.75">
@@ -11326,7 +11330,7 @@
       <c r="B189" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C189" s="7"/>
+      <c r="C189" s="8"/>
     </row>
     <row r="190" spans="1:8" ht="15.75">
       <c r="A190" s="1">
@@ -11335,7 +11339,7 @@
       <c r="B190" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C190" s="8"/>
+      <c r="C190" s="9"/>
     </row>
     <row r="191" spans="1:8" ht="15.75">
       <c r="A191" s="1">
@@ -11344,7 +11348,7 @@
       <c r="B191" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C191" s="9"/>
+      <c r="C191" s="10"/>
     </row>
     <row r="192" spans="1:8" ht="15.75">
       <c r="A192" s="1">
@@ -11353,7 +11357,7 @@
       <c r="B192" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C192" s="7"/>
+      <c r="C192" s="8"/>
     </row>
     <row r="193" spans="1:3" ht="15.75">
       <c r="A193" s="1">
@@ -11362,7 +11366,7 @@
       <c r="B193" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C193" s="8"/>
+      <c r="C193" s="9"/>
     </row>
     <row r="194" spans="1:3" ht="15.75">
       <c r="A194" s="1">
@@ -11371,7 +11375,7 @@
       <c r="B194" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C194" s="9"/>
+      <c r="C194" s="10"/>
     </row>
     <row r="195" spans="1:3" ht="15.75">
       <c r="A195" s="1">
@@ -11380,7 +11384,7 @@
       <c r="B195" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C195" s="7"/>
+      <c r="C195" s="8"/>
     </row>
     <row r="196" spans="1:3" ht="15.75">
       <c r="A196" s="1">
@@ -11389,7 +11393,7 @@
       <c r="B196" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C196" s="8"/>
+      <c r="C196" s="9"/>
     </row>
     <row r="197" spans="1:3" ht="15.75">
       <c r="A197" s="1">
@@ -11398,7 +11402,7 @@
       <c r="B197" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C197" s="9"/>
+      <c r="C197" s="10"/>
     </row>
     <row r="198" spans="1:3" ht="15.75">
       <c r="A198" s="1">
@@ -11407,7 +11411,7 @@
       <c r="B198" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C198" s="7"/>
+      <c r="C198" s="8"/>
     </row>
     <row r="199" spans="1:3" ht="15.75">
       <c r="A199" s="1">
@@ -11416,7 +11420,7 @@
       <c r="B199" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C199" s="8"/>
+      <c r="C199" s="9"/>
     </row>
     <row r="200" spans="1:3" ht="15.75">
       <c r="A200" s="1">
@@ -11425,7 +11429,7 @@
       <c r="B200" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C200" s="9"/>
+      <c r="C200" s="10"/>
     </row>
     <row r="201" spans="1:3" ht="15.75">
       <c r="A201" s="1">
@@ -11434,7 +11438,7 @@
       <c r="B201" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C201" s="7">
+      <c r="C201" s="8">
         <v>45051</v>
       </c>
     </row>
@@ -11445,7 +11449,7 @@
       <c r="B202" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C202" s="8"/>
+      <c r="C202" s="9"/>
     </row>
     <row r="203" spans="1:3" ht="15.75">
       <c r="A203" s="1">
@@ -11454,7 +11458,7 @@
       <c r="B203" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C203" s="9"/>
+      <c r="C203" s="10"/>
     </row>
     <row r="204" spans="1:3" ht="15.75">
       <c r="A204" s="1">
@@ -11463,7 +11467,7 @@
       <c r="B204" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C204" s="7">
+      <c r="C204" s="8">
         <v>45052</v>
       </c>
     </row>
@@ -11474,7 +11478,7 @@
       <c r="B205" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C205" s="8"/>
+      <c r="C205" s="9"/>
     </row>
     <row r="206" spans="1:3" ht="15.75">
       <c r="A206" s="1">
@@ -11483,7 +11487,7 @@
       <c r="B206" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C206" s="9"/>
+      <c r="C206" s="10"/>
     </row>
     <row r="207" spans="1:3" ht="15.75">
       <c r="A207" s="1">
@@ -11492,7 +11496,7 @@
       <c r="B207" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C207" s="7">
+      <c r="C207" s="8">
         <v>45053</v>
       </c>
     </row>
@@ -11503,7 +11507,7 @@
       <c r="B208" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C208" s="8"/>
+      <c r="C208" s="9"/>
     </row>
     <row r="209" spans="1:3" ht="15.75">
       <c r="A209" s="1">
@@ -11512,7 +11516,7 @@
       <c r="B209" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C209" s="9"/>
+      <c r="C209" s="10"/>
     </row>
     <row r="210" spans="1:3" ht="15.75">
       <c r="A210" s="1">
@@ -11521,7 +11525,7 @@
       <c r="B210" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C210" s="7">
+      <c r="C210" s="8">
         <v>45054</v>
       </c>
     </row>
@@ -11532,7 +11536,7 @@
       <c r="B211" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C211" s="8"/>
+      <c r="C211" s="9"/>
     </row>
     <row r="212" spans="1:3" ht="15.75">
       <c r="A212" s="1">
@@ -11541,7 +11545,7 @@
       <c r="B212" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C212" s="9"/>
+      <c r="C212" s="10"/>
     </row>
     <row r="213" spans="1:3" ht="15.75">
       <c r="A213" s="1">
@@ -11550,7 +11554,7 @@
       <c r="B213" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C213" s="7"/>
+      <c r="C213" s="8"/>
     </row>
     <row r="214" spans="1:3" ht="15.75">
       <c r="A214" s="1">
@@ -11559,7 +11563,7 @@
       <c r="B214" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C214" s="8"/>
+      <c r="C214" s="9"/>
     </row>
     <row r="215" spans="1:3" ht="15.75">
       <c r="A215" s="1">
@@ -11568,7 +11572,7 @@
       <c r="B215" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C215" s="9"/>
+      <c r="C215" s="10"/>
     </row>
     <row r="216" spans="1:3" ht="15.75">
       <c r="A216" s="1">
@@ -11577,7 +11581,7 @@
       <c r="B216" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C216" s="7">
+      <c r="C216" s="8">
         <v>45056</v>
       </c>
     </row>
@@ -11588,7 +11592,7 @@
       <c r="B217" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C217" s="8"/>
+      <c r="C217" s="9"/>
     </row>
     <row r="218" spans="1:3" ht="15.75">
       <c r="A218" s="1">
@@ -11597,170 +11601,170 @@
       <c r="B218" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C218" s="9"/>
+      <c r="C218" s="10"/>
     </row>
     <row r="219" spans="1:3" ht="15.75">
-      <c r="A219" s="18">
+      <c r="A219" s="1">
         <v>218</v>
       </c>
       <c r="B219" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C219" s="19">
+      <c r="C219" s="8">
         <v>45057</v>
       </c>
     </row>
     <row r="220" spans="1:3" ht="15.75">
-      <c r="A220" s="18">
+      <c r="A220" s="1">
         <v>219</v>
       </c>
       <c r="B220" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="C220" s="20"/>
+      <c r="C220" s="18"/>
     </row>
     <row r="221" spans="1:3" ht="15.75">
-      <c r="A221" s="18">
+      <c r="A221" s="1">
         <v>220</v>
       </c>
       <c r="B221" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="C221" s="20"/>
+      <c r="C221" s="18"/>
     </row>
     <row r="222" spans="1:3" ht="15.75">
-      <c r="A222" s="18">
+      <c r="A222" s="1">
         <v>221</v>
       </c>
       <c r="B222" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="C222" s="21"/>
+      <c r="C222" s="19"/>
     </row>
     <row r="223" spans="1:3" ht="15.75">
-      <c r="A223" s="18">
+      <c r="A223" s="1">
         <v>222</v>
       </c>
       <c r="B223" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="C223" s="19">
+      <c r="C223" s="8">
         <v>45058</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="15.75">
-      <c r="A224" s="18">
+      <c r="A224" s="1">
         <v>223</v>
       </c>
       <c r="B224" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="C224" s="22"/>
+      <c r="C224" s="9"/>
     </row>
     <row r="225" spans="1:3" ht="15.75">
-      <c r="A225" s="18">
+      <c r="A225" s="1">
         <v>224</v>
       </c>
       <c r="B225" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C225" s="23"/>
+      <c r="C225" s="10"/>
     </row>
     <row r="226" spans="1:3" ht="15.75">
-      <c r="A226" s="18">
+      <c r="A226" s="1">
         <v>225</v>
       </c>
       <c r="B226" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="C226" s="19">
+      <c r="C226" s="8">
         <v>45059</v>
       </c>
     </row>
     <row r="227" spans="1:3" ht="15.75">
-      <c r="A227" s="18">
+      <c r="A227" s="1">
         <v>226</v>
       </c>
       <c r="B227" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="C227" s="22"/>
+      <c r="C227" s="9"/>
     </row>
     <row r="228" spans="1:3" ht="15.75">
-      <c r="A228" s="18">
+      <c r="A228" s="1">
         <v>227</v>
       </c>
       <c r="B228" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="C228" s="23"/>
+      <c r="C228" s="10"/>
     </row>
     <row r="229" spans="1:3" ht="15.75">
-      <c r="A229" s="18">
+      <c r="A229" s="1">
         <v>228</v>
       </c>
       <c r="B229" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="C229" s="19">
+      <c r="C229" s="8">
         <v>45060</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="15.75">
-      <c r="A230" s="18">
+      <c r="A230" s="1">
         <v>229</v>
       </c>
       <c r="B230" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="C230" s="22"/>
+      <c r="C230" s="9"/>
     </row>
     <row r="231" spans="1:3" ht="15.75">
-      <c r="A231" s="18">
+      <c r="A231" s="1">
         <v>230</v>
       </c>
       <c r="B231" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="C231" s="23"/>
+      <c r="C231" s="10"/>
     </row>
     <row r="232" spans="1:3" ht="15.75">
-      <c r="A232" s="18">
+      <c r="A232" s="1">
         <v>231</v>
       </c>
       <c r="B232" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="C232" s="19">
+      <c r="C232" s="8">
         <v>45061</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="15.75">
-      <c r="A233" s="18">
+      <c r="A233" s="1">
         <v>232</v>
       </c>
       <c r="B233" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="C233" s="22"/>
+      <c r="C233" s="9"/>
     </row>
     <row r="234" spans="1:3" ht="15.75">
-      <c r="A234" s="18">
+      <c r="A234" s="1">
         <v>233</v>
       </c>
       <c r="B234" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="C234" s="23"/>
+      <c r="C234" s="10"/>
     </row>
     <row r="235" spans="1:3" ht="15.75">
       <c r="A235" s="1">
         <v>234</v>
       </c>
-      <c r="B235" s="17" t="s">
+      <c r="B235" s="20" t="s">
         <v>234</v>
       </c>
-      <c r="C235" s="7">
+      <c r="C235" s="8">
         <v>45062</v>
       </c>
     </row>
@@ -11768,28 +11772,28 @@
       <c r="A236" s="1">
         <v>235</v>
       </c>
-      <c r="B236" s="17" t="s">
+      <c r="B236" s="20" t="s">
         <v>235</v>
       </c>
-      <c r="C236" s="8"/>
+      <c r="C236" s="9"/>
     </row>
     <row r="237" spans="1:3" ht="15.75">
       <c r="A237" s="1">
         <v>236</v>
       </c>
-      <c r="B237" s="17" t="s">
+      <c r="B237" s="20" t="s">
         <v>236</v>
       </c>
-      <c r="C237" s="9"/>
+      <c r="C237" s="10"/>
     </row>
     <row r="238" spans="1:3" ht="15.75">
       <c r="A238" s="1">
         <v>237</v>
       </c>
-      <c r="B238" s="17" t="s">
+      <c r="B238" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="C238" s="7">
+      <c r="C238" s="8">
         <v>45063</v>
       </c>
     </row>
@@ -11797,28 +11801,28 @@
       <c r="A239" s="1">
         <v>238</v>
       </c>
-      <c r="B239" s="17" t="s">
+      <c r="B239" s="20" t="s">
         <v>238</v>
       </c>
-      <c r="C239" s="8"/>
+      <c r="C239" s="9"/>
     </row>
     <row r="240" spans="1:3" ht="15.75">
       <c r="A240" s="1">
         <v>239</v>
       </c>
-      <c r="B240" s="17" t="s">
+      <c r="B240" s="20" t="s">
         <v>239</v>
       </c>
-      <c r="C240" s="9"/>
+      <c r="C240" s="10"/>
     </row>
     <row r="241" spans="1:3" ht="15.75">
       <c r="A241" s="1">
         <v>240</v>
       </c>
-      <c r="B241" s="17" t="s">
+      <c r="B241" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="C241" s="7">
+      <c r="C241" s="8">
         <v>45064</v>
       </c>
     </row>
@@ -11826,28 +11830,28 @@
       <c r="A242" s="1">
         <v>241</v>
       </c>
-      <c r="B242" s="17" t="s">
+      <c r="B242" s="20" t="s">
         <v>241</v>
       </c>
-      <c r="C242" s="8"/>
+      <c r="C242" s="9"/>
     </row>
     <row r="243" spans="1:3" ht="15.75">
       <c r="A243" s="1">
         <v>242</v>
       </c>
-      <c r="B243" s="17" t="s">
+      <c r="B243" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="C243" s="9"/>
+      <c r="C243" s="10"/>
     </row>
     <row r="244" spans="1:3" ht="15.75">
       <c r="A244" s="1">
         <v>243</v>
       </c>
-      <c r="B244" s="2" t="s">
+      <c r="B244" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="C244" s="7">
+      <c r="C244" s="8">
         <v>45065</v>
       </c>
     </row>
@@ -11855,28 +11859,28 @@
       <c r="A245" s="1">
         <v>244</v>
       </c>
-      <c r="B245" s="2" t="s">
+      <c r="B245" s="20" t="s">
         <v>244</v>
       </c>
-      <c r="C245" s="8"/>
+      <c r="C245" s="9"/>
     </row>
     <row r="246" spans="1:3" ht="15.75">
       <c r="A246" s="1">
         <v>245</v>
       </c>
-      <c r="B246" s="2" t="s">
+      <c r="B246" s="20" t="s">
         <v>245</v>
       </c>
-      <c r="C246" s="9"/>
+      <c r="C246" s="10"/>
     </row>
     <row r="247" spans="1:3" ht="15.75">
       <c r="A247" s="1">
         <v>246</v>
       </c>
-      <c r="B247" s="2" t="s">
+      <c r="B247" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="C247" s="7">
+      <c r="C247" s="8">
         <v>45066</v>
       </c>
     </row>
@@ -11884,28 +11888,28 @@
       <c r="A248" s="1">
         <v>247</v>
       </c>
-      <c r="B248" s="2" t="s">
+      <c r="B248" s="20" t="s">
         <v>247</v>
       </c>
-      <c r="C248" s="8"/>
+      <c r="C248" s="9"/>
     </row>
     <row r="249" spans="1:3" ht="15.75">
       <c r="A249" s="1">
         <v>248</v>
       </c>
-      <c r="B249" s="2" t="s">
+      <c r="B249" s="20" t="s">
         <v>248</v>
       </c>
-      <c r="C249" s="9"/>
+      <c r="C249" s="10"/>
     </row>
     <row r="250" spans="1:3" ht="15.75">
       <c r="A250" s="1">
         <v>249</v>
       </c>
-      <c r="B250" s="2" t="s">
+      <c r="B250" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="C250" s="7">
+      <c r="C250" s="8">
         <v>45067</v>
       </c>
     </row>
@@ -11913,28 +11917,28 @@
       <c r="A251" s="1">
         <v>250</v>
       </c>
-      <c r="B251" s="2" t="s">
+      <c r="B251" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="C251" s="8"/>
+      <c r="C251" s="9"/>
     </row>
     <row r="252" spans="1:3" ht="15.75">
       <c r="A252" s="1">
         <v>251</v>
       </c>
-      <c r="B252" s="2" t="s">
+      <c r="B252" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="C252" s="9"/>
+      <c r="C252" s="10"/>
     </row>
     <row r="253" spans="1:3" ht="15.75">
       <c r="A253" s="1">
         <v>252</v>
       </c>
-      <c r="B253" s="2" t="s">
+      <c r="B253" s="21" t="s">
         <v>252</v>
       </c>
-      <c r="C253" s="7">
+      <c r="C253" s="8">
         <v>45068</v>
       </c>
     </row>
@@ -11942,28 +11946,28 @@
       <c r="A254" s="1">
         <v>253</v>
       </c>
-      <c r="B254" s="2" t="s">
+      <c r="B254" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="C254" s="8"/>
+      <c r="C254" s="9"/>
     </row>
     <row r="255" spans="1:3" ht="15.75">
       <c r="A255" s="1">
         <v>254</v>
       </c>
-      <c r="B255" s="2" t="s">
+      <c r="B255" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="C255" s="9"/>
+      <c r="C255" s="10"/>
     </row>
     <row r="256" spans="1:3" ht="15.75">
       <c r="A256" s="1">
         <v>255</v>
       </c>
-      <c r="B256" s="2" t="s">
+      <c r="B256" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="C256" s="7">
+      <c r="C256" s="8">
         <v>45069</v>
       </c>
     </row>
@@ -11971,28 +11975,28 @@
       <c r="A257" s="1">
         <v>256</v>
       </c>
-      <c r="B257" s="2" t="s">
+      <c r="B257" s="21" t="s">
         <v>256</v>
       </c>
-      <c r="C257" s="8"/>
+      <c r="C257" s="9"/>
     </row>
     <row r="258" spans="1:3" ht="15.75">
       <c r="A258" s="1">
         <v>257</v>
       </c>
-      <c r="B258" s="2" t="s">
+      <c r="B258" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="C258" s="9"/>
+      <c r="C258" s="10"/>
     </row>
     <row r="259" spans="1:3" ht="15.75">
       <c r="A259" s="1">
         <v>258</v>
       </c>
-      <c r="B259" s="2" t="s">
+      <c r="B259" s="21" t="s">
         <v>258</v>
       </c>
-      <c r="C259" s="7">
+      <c r="C259" s="8">
         <v>45070</v>
       </c>
     </row>
@@ -12000,19 +12004,19 @@
       <c r="A260" s="1">
         <v>259</v>
       </c>
-      <c r="B260" s="2" t="s">
+      <c r="B260" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="C260" s="8"/>
+      <c r="C260" s="9"/>
     </row>
     <row r="261" spans="1:3" ht="15.75">
       <c r="A261" s="1">
         <v>260</v>
       </c>
-      <c r="B261" s="2" t="s">
+      <c r="B261" s="21" t="s">
         <v>260</v>
       </c>
-      <c r="C261" s="9"/>
+      <c r="C261" s="10"/>
     </row>
     <row r="262" spans="1:3" ht="15.75">
       <c r="A262" s="1">
@@ -12021,7 +12025,7 @@
       <c r="B262" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C262" s="7">
+      <c r="C262" s="8">
         <v>45071</v>
       </c>
     </row>
@@ -12032,7 +12036,7 @@
       <c r="B263" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C263" s="8"/>
+      <c r="C263" s="9"/>
     </row>
     <row r="264" spans="1:3" ht="15.75">
       <c r="A264" s="1">
@@ -12041,7 +12045,7 @@
       <c r="B264" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C264" s="9"/>
+      <c r="C264" s="10"/>
     </row>
     <row r="265" spans="1:3" ht="15.75">
       <c r="A265" s="1">
@@ -12050,7 +12054,7 @@
       <c r="B265" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C265" s="7">
+      <c r="C265" s="8">
         <v>45072</v>
       </c>
     </row>
@@ -12061,7 +12065,7 @@
       <c r="B266" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C266" s="8"/>
+      <c r="C266" s="9"/>
     </row>
     <row r="267" spans="1:3" ht="15.75">
       <c r="A267" s="1">
@@ -12070,7 +12074,7 @@
       <c r="B267" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C267" s="9"/>
+      <c r="C267" s="10"/>
     </row>
     <row r="268" spans="1:3" ht="15.75">
       <c r="A268" s="1">
@@ -12079,7 +12083,7 @@
       <c r="B268" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="C268" s="7">
+      <c r="C268" s="8">
         <v>45073</v>
       </c>
     </row>
@@ -12090,7 +12094,7 @@
       <c r="B269" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="C269" s="8"/>
+      <c r="C269" s="9"/>
     </row>
     <row r="270" spans="1:3" ht="15.75">
       <c r="A270" s="1">
@@ -12099,7 +12103,7 @@
       <c r="B270" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C270" s="9"/>
+      <c r="C270" s="10"/>
     </row>
     <row r="271" spans="1:3" ht="15.75">
       <c r="A271" s="1">
@@ -12108,7 +12112,7 @@
       <c r="B271" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="C271" s="7">
+      <c r="C271" s="8">
         <v>45074</v>
       </c>
     </row>
@@ -12119,7 +12123,7 @@
       <c r="B272" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C272" s="8"/>
+      <c r="C272" s="9"/>
     </row>
     <row r="273" spans="1:3" ht="15.75">
       <c r="A273" s="1">
@@ -12128,7 +12132,7 @@
       <c r="B273" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C273" s="9"/>
+      <c r="C273" s="10"/>
     </row>
     <row r="274" spans="1:3" ht="15.75">
       <c r="A274" s="1">
@@ -12137,7 +12141,7 @@
       <c r="B274" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="C274" s="7">
+      <c r="C274" s="8">
         <v>45075</v>
       </c>
     </row>
@@ -12148,7 +12152,7 @@
       <c r="B275" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C275" s="8"/>
+      <c r="C275" s="9"/>
     </row>
     <row r="276" spans="1:3" ht="15.75">
       <c r="A276" s="1">
@@ -12157,7 +12161,7 @@
       <c r="B276" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="C276" s="9"/>
+      <c r="C276" s="10"/>
     </row>
     <row r="277" spans="1:3" ht="15.75">
       <c r="A277" s="1">
@@ -12166,7 +12170,7 @@
       <c r="B277" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="C277" s="7">
+      <c r="C277" s="8">
         <v>45076</v>
       </c>
     </row>
@@ -12177,7 +12181,7 @@
       <c r="B278" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C278" s="8"/>
+      <c r="C278" s="9"/>
     </row>
     <row r="279" spans="1:3" ht="15.75">
       <c r="A279" s="1">
@@ -12186,7 +12190,7 @@
       <c r="B279" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C279" s="9"/>
+      <c r="C279" s="10"/>
     </row>
     <row r="280" spans="1:3" ht="15.75">
       <c r="A280" s="1">
@@ -12195,7 +12199,7 @@
       <c r="B280" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="C280" s="7">
+      <c r="C280" s="8">
         <v>45077</v>
       </c>
     </row>
@@ -12206,7 +12210,7 @@
       <c r="B281" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C281" s="8"/>
+      <c r="C281" s="9"/>
     </row>
     <row r="282" spans="1:3" ht="15.75">
       <c r="A282" s="1">
@@ -12215,7 +12219,7 @@
       <c r="B282" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C282" s="9"/>
+      <c r="C282" s="10"/>
     </row>
     <row r="283" spans="1:3" ht="15.75">
       <c r="A283" s="1">
@@ -12224,7 +12228,7 @@
       <c r="B283" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C283" s="7">
+      <c r="C283" s="8">
         <v>45078</v>
       </c>
     </row>
@@ -12235,7 +12239,7 @@
       <c r="B284" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="C284" s="8"/>
+      <c r="C284" s="9"/>
     </row>
     <row r="285" spans="1:3" ht="15.75">
       <c r="A285" s="1">
@@ -12244,7 +12248,7 @@
       <c r="B285" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C285" s="9"/>
+      <c r="C285" s="10"/>
     </row>
     <row r="286" spans="1:3" ht="15.75">
       <c r="A286" s="1">
@@ -12253,7 +12257,7 @@
       <c r="B286" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="C286" s="7">
+      <c r="C286" s="8">
         <v>45079</v>
       </c>
     </row>
@@ -12264,7 +12268,7 @@
       <c r="B287" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="C287" s="8"/>
+      <c r="C287" s="9"/>
     </row>
     <row r="288" spans="1:3" ht="15.75">
       <c r="A288" s="1">
@@ -12273,7 +12277,7 @@
       <c r="B288" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="C288" s="9"/>
+      <c r="C288" s="10"/>
     </row>
     <row r="289" spans="1:3" ht="15.75">
       <c r="A289" s="1">
@@ -12282,7 +12286,7 @@
       <c r="B289" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C289" s="7">
+      <c r="C289" s="8">
         <v>45080</v>
       </c>
     </row>
@@ -12293,7 +12297,7 @@
       <c r="B290" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C290" s="8"/>
+      <c r="C290" s="9"/>
     </row>
     <row r="291" spans="1:3" ht="15.75">
       <c r="A291" s="1">
@@ -12302,7 +12306,7 @@
       <c r="B291" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="C291" s="9"/>
+      <c r="C291" s="10"/>
     </row>
     <row r="292" spans="1:3" ht="15.75">
       <c r="A292" s="1">
@@ -12311,7 +12315,7 @@
       <c r="B292" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="C292" s="7">
+      <c r="C292" s="8">
         <v>45081</v>
       </c>
     </row>
@@ -12322,7 +12326,7 @@
       <c r="B293" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="C293" s="8"/>
+      <c r="C293" s="9"/>
     </row>
     <row r="294" spans="1:3" ht="15.75">
       <c r="A294" s="1">
@@ -12331,7 +12335,7 @@
       <c r="B294" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C294" s="9"/>
+      <c r="C294" s="10"/>
     </row>
     <row r="295" spans="1:3" ht="15.75">
       <c r="A295" s="1">
@@ -12340,7 +12344,7 @@
       <c r="B295" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C295" s="7">
+      <c r="C295" s="8">
         <v>45082</v>
       </c>
     </row>
@@ -12351,7 +12355,7 @@
       <c r="B296" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="C296" s="8"/>
+      <c r="C296" s="9"/>
     </row>
     <row r="297" spans="1:3" ht="15.75">
       <c r="A297" s="1">
@@ -12360,7 +12364,7 @@
       <c r="B297" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="C297" s="9"/>
+      <c r="C297" s="10"/>
     </row>
     <row r="298" spans="1:3" ht="15.75">
       <c r="A298" s="1">
@@ -12369,7 +12373,7 @@
       <c r="B298" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="C298" s="7">
+      <c r="C298" s="8">
         <v>45083</v>
       </c>
     </row>
@@ -12380,7 +12384,7 @@
       <c r="B299" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C299" s="8"/>
+      <c r="C299" s="9"/>
     </row>
     <row r="300" spans="1:3" ht="15.75">
       <c r="A300" s="1">
@@ -12389,7 +12393,7 @@
       <c r="B300" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C300" s="9"/>
+      <c r="C300" s="10"/>
     </row>
     <row r="301" spans="1:3" ht="15.75">
       <c r="A301" s="1">
@@ -36702,52 +36706,23 @@
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="C238:C240"/>
-    <mergeCell ref="C241:C243"/>
-    <mergeCell ref="C244:C246"/>
-    <mergeCell ref="C247:C249"/>
-    <mergeCell ref="C223:C225"/>
-    <mergeCell ref="C226:C228"/>
-    <mergeCell ref="C229:C231"/>
-    <mergeCell ref="C232:C234"/>
-    <mergeCell ref="C235:C237"/>
-    <mergeCell ref="C120:C125"/>
-    <mergeCell ref="C111:C113"/>
-    <mergeCell ref="C138:C140"/>
-    <mergeCell ref="C141:C143"/>
-    <mergeCell ref="C135:C137"/>
-    <mergeCell ref="C126:C131"/>
-    <mergeCell ref="C132:C134"/>
-    <mergeCell ref="C108:C110"/>
-    <mergeCell ref="C105:C107"/>
-    <mergeCell ref="C102:C104"/>
-    <mergeCell ref="C99:C101"/>
-    <mergeCell ref="C114:C119"/>
-    <mergeCell ref="C48:C53"/>
-    <mergeCell ref="C96:C98"/>
-    <mergeCell ref="C90:C95"/>
-    <mergeCell ref="C84:C89"/>
-    <mergeCell ref="C78:C83"/>
-    <mergeCell ref="C72:C77"/>
-    <mergeCell ref="C66:C71"/>
-    <mergeCell ref="C60:C65"/>
-    <mergeCell ref="C54:C59"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="C2:C11"/>
-    <mergeCell ref="C12:C21"/>
-    <mergeCell ref="C22:C31"/>
-    <mergeCell ref="C32:C41"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="C153:C155"/>
-    <mergeCell ref="C144:C146"/>
-    <mergeCell ref="C150:C152"/>
-    <mergeCell ref="C147:C149"/>
-    <mergeCell ref="C171:C173"/>
-    <mergeCell ref="C156:C158"/>
-    <mergeCell ref="C159:C161"/>
-    <mergeCell ref="C162:C164"/>
-    <mergeCell ref="C165:C167"/>
-    <mergeCell ref="C168:C170"/>
+    <mergeCell ref="C295:C297"/>
+    <mergeCell ref="C298:C300"/>
+    <mergeCell ref="C280:C282"/>
+    <mergeCell ref="C283:C285"/>
+    <mergeCell ref="C286:C288"/>
+    <mergeCell ref="C289:C291"/>
+    <mergeCell ref="C292:C294"/>
+    <mergeCell ref="C265:C267"/>
+    <mergeCell ref="C268:C270"/>
+    <mergeCell ref="C271:C273"/>
+    <mergeCell ref="C274:C276"/>
+    <mergeCell ref="C277:C279"/>
+    <mergeCell ref="C250:C252"/>
+    <mergeCell ref="C253:C255"/>
+    <mergeCell ref="C256:C258"/>
+    <mergeCell ref="C259:C261"/>
+    <mergeCell ref="C262:C264"/>
     <mergeCell ref="C219:C222"/>
     <mergeCell ref="C204:C206"/>
     <mergeCell ref="C207:C209"/>
@@ -36764,23 +36739,52 @@
     <mergeCell ref="C195:C197"/>
     <mergeCell ref="C213:C215"/>
     <mergeCell ref="C216:C218"/>
-    <mergeCell ref="C250:C252"/>
-    <mergeCell ref="C253:C255"/>
-    <mergeCell ref="C256:C258"/>
-    <mergeCell ref="C259:C261"/>
-    <mergeCell ref="C262:C264"/>
-    <mergeCell ref="C265:C267"/>
-    <mergeCell ref="C268:C270"/>
-    <mergeCell ref="C271:C273"/>
-    <mergeCell ref="C274:C276"/>
-    <mergeCell ref="C277:C279"/>
-    <mergeCell ref="C295:C297"/>
-    <mergeCell ref="C298:C300"/>
-    <mergeCell ref="C280:C282"/>
-    <mergeCell ref="C283:C285"/>
-    <mergeCell ref="C286:C288"/>
-    <mergeCell ref="C289:C291"/>
-    <mergeCell ref="C292:C294"/>
+    <mergeCell ref="C153:C155"/>
+    <mergeCell ref="C144:C146"/>
+    <mergeCell ref="C150:C152"/>
+    <mergeCell ref="C147:C149"/>
+    <mergeCell ref="C171:C173"/>
+    <mergeCell ref="C156:C158"/>
+    <mergeCell ref="C159:C161"/>
+    <mergeCell ref="C162:C164"/>
+    <mergeCell ref="C165:C167"/>
+    <mergeCell ref="C168:C170"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="C12:C21"/>
+    <mergeCell ref="C22:C31"/>
+    <mergeCell ref="C32:C41"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="C48:C53"/>
+    <mergeCell ref="C96:C98"/>
+    <mergeCell ref="C90:C95"/>
+    <mergeCell ref="C84:C89"/>
+    <mergeCell ref="C78:C83"/>
+    <mergeCell ref="C72:C77"/>
+    <mergeCell ref="C66:C71"/>
+    <mergeCell ref="C60:C65"/>
+    <mergeCell ref="C54:C59"/>
+    <mergeCell ref="C108:C110"/>
+    <mergeCell ref="C105:C107"/>
+    <mergeCell ref="C102:C104"/>
+    <mergeCell ref="C99:C101"/>
+    <mergeCell ref="C114:C119"/>
+    <mergeCell ref="C120:C125"/>
+    <mergeCell ref="C111:C113"/>
+    <mergeCell ref="C138:C140"/>
+    <mergeCell ref="C141:C143"/>
+    <mergeCell ref="C135:C137"/>
+    <mergeCell ref="C126:C131"/>
+    <mergeCell ref="C132:C134"/>
+    <mergeCell ref="C238:C240"/>
+    <mergeCell ref="C241:C243"/>
+    <mergeCell ref="C244:C246"/>
+    <mergeCell ref="C247:C249"/>
+    <mergeCell ref="C223:C225"/>
+    <mergeCell ref="C226:C228"/>
+    <mergeCell ref="C229:C231"/>
+    <mergeCell ref="C232:C234"/>
+    <mergeCell ref="C235:C237"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>